<commit_message>
Initial commit of capstone project with KPIs and analysis notebooks
</commit_message>
<xml_diff>
--- a/Updated_Activity_Data_With_KPIs.xlsx
+++ b/Updated_Activity_Data_With_KPIs.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI156"/>
+  <dimension ref="A1:AH156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,20 +595,15 @@
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Duration_Min</t>
+          <t>HR_Reserve_Ratio</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>HR_Reserve_Ratio</t>
+          <t>Calories_per_Km</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Calories_per_Km</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Calories_per_Speed</t>
         </is>
@@ -675,8 +670,10 @@
           <t>00:58:50</t>
         </is>
       </c>
-      <c r="Q2" t="n">
-        <v>753</v>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>753</t>
+        </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
@@ -729,15 +726,12 @@
         <v>5.338983050847458</v>
       </c>
       <c r="AF2" t="n">
-        <v>59</v>
+        <v>0.3839285714285715</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.3839285714285715</v>
+        <v>0.6665256030469742</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.6665256030469742</v>
-      </c>
-      <c r="AI2" t="n">
         <v>0.6554168429961912</v>
       </c>
     </row>
@@ -802,8 +796,10 @@
           <t>00:48:02</t>
         </is>
       </c>
-      <c r="Q3" t="n">
-        <v>626</v>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>626</t>
+        </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -856,15 +852,12 @@
         <v>5.104166666666667</v>
       </c>
       <c r="AF3" t="n">
-        <v>48</v>
+        <v>0.2803738317757009</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.2803738317757009</v>
+        <v>0.5177514792899408</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.5177514792899408</v>
-      </c>
-      <c r="AI3" t="n">
         <v>0.4142011834319527</v>
       </c>
     </row>
@@ -929,8 +922,10 @@
           <t>00:38:44</t>
         </is>
       </c>
-      <c r="Q4" t="n">
-        <v>528</v>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>528</t>
+        </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
@@ -983,15 +978,12 @@
         <v>5.2</v>
       </c>
       <c r="AF4" t="n">
-        <v>40</v>
+        <v>0.2293577981651376</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.2293577981651376</v>
+        <v>0.746054519368723</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.746054519368723</v>
-      </c>
-      <c r="AI4" t="n">
         <v>0.4973696795791487</v>
       </c>
     </row>
@@ -1056,8 +1048,10 @@
           <t>00:47:57</t>
         </is>
       </c>
-      <c r="Q5" t="n">
-        <v>661</v>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>661</t>
+        </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
@@ -1110,15 +1104,12 @@
         <v>5.125</v>
       </c>
       <c r="AF5" t="n">
-        <v>48</v>
+        <v>0.3545454545454546</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.3545454545454546</v>
+        <v>0.5216284987277353</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.5216284987277353</v>
-      </c>
-      <c r="AI5" t="n">
         <v>0.4173027989821883</v>
       </c>
     </row>
@@ -1183,8 +1174,10 @@
           <t>00:47:04</t>
         </is>
       </c>
-      <c r="Q6" t="n">
-        <v>619</v>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>619</t>
+        </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
@@ -1237,15 +1230,12 @@
         <v>5.23404255319149</v>
       </c>
       <c r="AF6" t="n">
-        <v>47</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.3846153846153846</v>
+        <v>0.4973716134249899</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.4973716134249899</v>
-      </c>
-      <c r="AI6" t="n">
         <v>0.3896077638495754</v>
       </c>
     </row>
@@ -1310,8 +1300,10 @@
           <t>00:47:20</t>
         </is>
       </c>
-      <c r="Q7" t="n">
-        <v>638</v>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>638</t>
+        </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
@@ -1364,15 +1356,12 @@
         <v>4.979166666666667</v>
       </c>
       <c r="AF7" t="n">
-        <v>48</v>
+        <v>0.2924528301886792</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.2924528301886792</v>
+        <v>0.4962624584717608</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.4962624584717608</v>
-      </c>
-      <c r="AI7" t="n">
         <v>0.3970099667774086</v>
       </c>
     </row>
@@ -1437,8 +1426,10 @@
           <t>01:04:53</t>
         </is>
       </c>
-      <c r="Q8" t="n">
-        <v>821</v>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>821</t>
+        </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
@@ -1491,15 +1482,12 @@
         <v>3.876923076923077</v>
       </c>
       <c r="AF8" t="n">
-        <v>65</v>
+        <v>0.29</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.29</v>
+        <v>0.5305263157894737</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.5305263157894737</v>
-      </c>
-      <c r="AI8" t="n">
         <v>0.5747368421052631</v>
       </c>
     </row>
@@ -1564,8 +1552,10 @@
           <t>00:37:22</t>
         </is>
       </c>
-      <c r="Q9" t="n">
-        <v>515</v>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>515</t>
+        </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
@@ -1618,15 +1608,12 @@
         <v>5.648648648648648</v>
       </c>
       <c r="AF9" t="n">
-        <v>37</v>
+        <v>0.2803738317757009</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.2803738317757009</v>
+        <v>0.4561326931470974</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.4561326931470974</v>
-      </c>
-      <c r="AI9" t="n">
         <v>0.2812818274407101</v>
       </c>
     </row>
@@ -1691,7 +1678,11 @@
           <t>01:27:56</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>1,102</t>
+        </is>
+      </c>
       <c r="R10" t="inlineStr">
         <is>
           <t>Vivoactive HR 4.0.0.0</t>
@@ -1743,15 +1734,12 @@
         <v>5.769230769230769</v>
       </c>
       <c r="AF10" t="n">
-        <v>91</v>
+        <v>0.22</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.22</v>
+        <v>0.7747933884297521</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.7747933884297521</v>
-      </c>
-      <c r="AI10" t="n">
         <v>1.175103305785124</v>
       </c>
     </row>
@@ -1816,8 +1804,10 @@
           <t>01:07:58</t>
         </is>
       </c>
-      <c r="Q11" t="n">
-        <v>941</v>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>941</t>
+        </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
@@ -1870,15 +1860,12 @@
         <v>4.623188405797102</v>
       </c>
       <c r="AF11" t="n">
-        <v>69</v>
+        <v>0.5096153846153846</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.5096153846153846</v>
+        <v>0.6872037914691943</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.6872037914691943</v>
-      </c>
-      <c r="AI11" t="n">
         <v>0.7902843601895734</v>
       </c>
     </row>
@@ -1943,8 +1930,10 @@
           <t>00:43:50</t>
         </is>
       </c>
-      <c r="Q12" t="n">
-        <v>668</v>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>668</t>
+        </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
@@ -1997,15 +1986,12 @@
         <v>4.377777777777778</v>
       </c>
       <c r="AF12" t="n">
-        <v>45</v>
+        <v>0.1509433962264151</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.1509433962264151</v>
+        <v>0.4497716894977169</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.4497716894977169</v>
-      </c>
-      <c r="AI12" t="n">
         <v>0.3373287671232877</v>
       </c>
     </row>
@@ -2070,8 +2056,10 @@
           <t>00:39:07</t>
         </is>
       </c>
-      <c r="Q13" t="n">
-        <v>573</v>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>573</t>
+        </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
@@ -2124,15 +2112,12 @@
         <v>5.589743589743589</v>
       </c>
       <c r="AF13" t="n">
-        <v>39</v>
+        <v>0.22</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.22</v>
+        <v>0.4861730597680642</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.4861730597680642</v>
-      </c>
-      <c r="AI13" t="n">
         <v>0.3160124888492418</v>
       </c>
     </row>
@@ -2197,8 +2182,10 @@
           <t>00:36:37</t>
         </is>
       </c>
-      <c r="Q14" t="n">
-        <v>562</v>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>562</t>
+        </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
@@ -2251,15 +2238,12 @@
         <v>5.578947368421052</v>
       </c>
       <c r="AF14" t="n">
-        <v>38</v>
+        <v>0.2524271844660194</v>
       </c>
       <c r="AG14" t="n">
-        <v>0.2524271844660194</v>
+        <v>0.457685664939551</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.457685664939551</v>
-      </c>
-      <c r="AI14" t="n">
         <v>0.289867587795049</v>
       </c>
     </row>
@@ -2324,8 +2308,10 @@
           <t>00:30:00</t>
         </is>
       </c>
-      <c r="Q15" t="n">
-        <v>304</v>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>304</t>
+        </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
@@ -2378,15 +2364,12 @@
         <v>0.1</v>
       </c>
       <c r="AF15" t="n">
-        <v>30</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.07692307692307693</v>
+        <v>0.0154639175257732</v>
       </c>
       <c r="AH15" t="n">
-        <v>0.0154639175257732</v>
-      </c>
-      <c r="AI15" t="n">
         <v>0.007731958762886598</v>
       </c>
     </row>
@@ -2451,8 +2434,10 @@
           <t>00:57:35</t>
         </is>
       </c>
-      <c r="Q16" t="n">
-        <v>768</v>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>768</t>
+        </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
@@ -2505,15 +2490,12 @@
         <v>0.4827586206896552</v>
       </c>
       <c r="AF16" t="n">
-        <v>58</v>
+        <v>0.6020408163265306</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.6020408163265306</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="AI16" t="n">
         <v>0.1342592592592593</v>
       </c>
     </row>
@@ -2578,8 +2560,10 @@
           <t>00:16:40</t>
         </is>
       </c>
-      <c r="Q17" t="n">
-        <v>226</v>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>226</t>
+        </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
@@ -2632,15 +2616,12 @@
         <v>0.4736842105263158</v>
       </c>
       <c r="AF17" t="n">
-        <v>19</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.303030303030303</v>
+        <v>0.04582484725050916</v>
       </c>
       <c r="AH17" t="n">
-        <v>0.04582484725050916</v>
-      </c>
-      <c r="AI17" t="n">
         <v>0.0145112016293279</v>
       </c>
     </row>
@@ -2705,8 +2686,10 @@
           <t>00:41:33</t>
         </is>
       </c>
-      <c r="Q18" t="n">
-        <v>583</v>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>583</t>
+        </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
@@ -2759,15 +2742,12 @@
         <v>0.09523809523809523</v>
       </c>
       <c r="AF18" t="n">
-        <v>42</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.3076923076923077</v>
+        <v>0.01972386587771203</v>
       </c>
       <c r="AH18" t="n">
-        <v>0.01972386587771203</v>
-      </c>
-      <c r="AI18" t="n">
         <v>0.01380670611439842</v>
       </c>
     </row>
@@ -2832,8 +2812,10 @@
           <t>00:20:11</t>
         </is>
       </c>
-      <c r="Q19" t="n">
-        <v>257</v>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>257</t>
+        </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
@@ -2886,15 +2868,12 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="AF19" t="n">
-        <v>21</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.01476377952755906</v>
       </c>
       <c r="AH19" t="n">
-        <v>0.01476377952755906</v>
-      </c>
-      <c r="AI19" t="n">
         <v>0.00516732283464567</v>
       </c>
     </row>
@@ -2959,8 +2938,10 @@
           <t>00:37:03</t>
         </is>
       </c>
-      <c r="Q20" t="n">
-        <v>498</v>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>498</t>
+        </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
@@ -3013,15 +2994,12 @@
         <v>5.447368421052632</v>
       </c>
       <c r="AF20" t="n">
-        <v>38</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.08823529411764706</v>
+        <v>0.4579646017699115</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.4579646017699115</v>
-      </c>
-      <c r="AI20" t="n">
         <v>0.2900442477876106</v>
       </c>
     </row>
@@ -3086,8 +3064,10 @@
           <t>00:49:27</t>
         </is>
       </c>
-      <c r="Q21" t="n">
-        <v>678</v>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>678</t>
+        </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
@@ -3140,15 +3120,12 @@
         <v>4.938775510204081</v>
       </c>
       <c r="AF21" t="n">
-        <v>49</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="AG21" t="n">
-        <v>0.2380952380952381</v>
+        <v>0.8692528735632185</v>
       </c>
       <c r="AH21" t="n">
-        <v>0.8692528735632185</v>
-      </c>
-      <c r="AI21" t="n">
         <v>0.7098898467432951</v>
       </c>
     </row>
@@ -3213,8 +3190,10 @@
           <t>00:36:50</t>
         </is>
       </c>
-      <c r="Q22" t="n">
-        <v>464</v>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>464</t>
+        </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
@@ -3267,15 +3246,12 @@
         <v>5.72972972972973</v>
       </c>
       <c r="AF22" t="n">
-        <v>37</v>
+        <v>0.2604166666666667</v>
       </c>
       <c r="AG22" t="n">
-        <v>0.2604166666666667</v>
+        <v>0.4820372896771259</v>
       </c>
       <c r="AH22" t="n">
-        <v>0.4820372896771259</v>
-      </c>
-      <c r="AI22" t="n">
         <v>0.2972563286342277</v>
       </c>
     </row>
@@ -3340,7 +3316,11 @@
           <t>01:35:25</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>1,263</t>
+        </is>
+      </c>
       <c r="R23" t="inlineStr">
         <is>
           <t>Vivoactive HR 3.90.0.0</t>
@@ -3392,15 +3372,12 @@
         <v>5.928571428571429</v>
       </c>
       <c r="AF23" t="n">
-        <v>98</v>
+        <v>0.3069306930693069</v>
       </c>
       <c r="AG23" t="n">
-        <v>0.3069306930693069</v>
+        <v>0.7954545454545455</v>
       </c>
       <c r="AH23" t="n">
-        <v>0.7954545454545455</v>
-      </c>
-      <c r="AI23" t="n">
         <v>1.299242424242424</v>
       </c>
     </row>
@@ -3465,8 +3442,10 @@
           <t>00:38:19</t>
         </is>
       </c>
-      <c r="Q24" t="n">
-        <v>542</v>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>542</t>
+        </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
@@ -3519,15 +3498,12 @@
         <v>5.358974358974359</v>
       </c>
       <c r="AF24" t="n">
-        <v>39</v>
+        <v>0.2551020408163265</v>
       </c>
       <c r="AG24" t="n">
-        <v>0.2551020408163265</v>
+        <v>0.4713576905728462</v>
       </c>
       <c r="AH24" t="n">
-        <v>0.4713576905728462</v>
-      </c>
-      <c r="AI24" t="n">
         <v>0.3063824988723501</v>
       </c>
     </row>
@@ -3592,8 +3568,10 @@
           <t>00:56:24</t>
         </is>
       </c>
-      <c r="Q25" t="n">
-        <v>833</v>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>833</t>
+        </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
@@ -3646,15 +3624,12 @@
         <v>5.428571428571429</v>
       </c>
       <c r="AF25" t="n">
-        <v>56</v>
+        <v>0.1869158878504673</v>
       </c>
       <c r="AG25" t="n">
-        <v>0.1869158878504673</v>
+        <v>1.091954022988506</v>
       </c>
       <c r="AH25" t="n">
-        <v>1.091954022988506</v>
-      </c>
-      <c r="AI25" t="n">
         <v>1.019157088122605</v>
       </c>
     </row>
@@ -3719,8 +3694,10 @@
           <t>00:37:39</t>
         </is>
       </c>
-      <c r="Q26" t="n">
-        <v>587</v>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>587</t>
+        </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
@@ -3773,15 +3750,12 @@
         <v>5.513513513513513</v>
       </c>
       <c r="AF26" t="n">
-        <v>37</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="AG26" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.4523281596452328</v>
       </c>
       <c r="AH26" t="n">
-        <v>0.4523281596452328</v>
-      </c>
-      <c r="AI26" t="n">
         <v>0.2789356984478936</v>
       </c>
     </row>
@@ -3846,8 +3820,10 @@
           <t>00:47:56</t>
         </is>
       </c>
-      <c r="Q27" t="n">
-        <v>767</v>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>767</t>
+        </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
@@ -3900,15 +3876,12 @@
         <v>5</v>
       </c>
       <c r="AF27" t="n">
-        <v>49</v>
+        <v>0.2647058823529412</v>
       </c>
       <c r="AG27" t="n">
-        <v>0.2647058823529412</v>
+        <v>0.5070364238410596</v>
       </c>
       <c r="AH27" t="n">
-        <v>0.5070364238410596</v>
-      </c>
-      <c r="AI27" t="n">
         <v>0.4140797461368654</v>
       </c>
     </row>
@@ -3973,8 +3946,10 @@
           <t>00:38:29</t>
         </is>
       </c>
-      <c r="Q28" t="n">
-        <v>405</v>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>405</t>
+        </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
@@ -4027,15 +4002,12 @@
         <v>0.3076923076923077</v>
       </c>
       <c r="AF28" t="n">
-        <v>39</v>
+        <v>0.7373737373737373</v>
       </c>
       <c r="AG28" t="n">
-        <v>0.7373737373737373</v>
+        <v>0.01635322976287817</v>
       </c>
       <c r="AH28" t="n">
-        <v>0.01635322976287817</v>
-      </c>
-      <c r="AI28" t="n">
         <v>0.01062959934587081</v>
       </c>
     </row>
@@ -4100,8 +4072,10 @@
           <t>00:49:43</t>
         </is>
       </c>
-      <c r="Q29" t="n">
-        <v>596</v>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>596</t>
+        </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
@@ -4154,15 +4128,12 @@
         <v>10.06122448979592</v>
       </c>
       <c r="AF29" t="n">
-        <v>49</v>
+        <v>0.1545454545454545</v>
       </c>
       <c r="AG29" t="n">
-        <v>0.1545454545454545</v>
+        <v>0.6872037914691943</v>
       </c>
       <c r="AH29" t="n">
-        <v>0.6872037914691943</v>
-      </c>
-      <c r="AI29" t="n">
         <v>0.561216429699842</v>
       </c>
     </row>
@@ -4227,8 +4198,10 @@
           <t>00:40:04</t>
         </is>
       </c>
-      <c r="Q30" t="n">
-        <v>435</v>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>435</t>
+        </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
@@ -4281,15 +4254,12 @@
         <v>5.25</v>
       </c>
       <c r="AF30" t="n">
-        <v>40</v>
+        <v>0.3163265306122449</v>
       </c>
       <c r="AG30" t="n">
-        <v>0.3163265306122449</v>
+        <v>0.4727600180099055</v>
       </c>
       <c r="AH30" t="n">
-        <v>0.4727600180099055</v>
-      </c>
-      <c r="AI30" t="n">
         <v>0.3151733453399369</v>
       </c>
     </row>
@@ -4354,7 +4324,11 @@
           <t>01:55:40</t>
         </is>
       </c>
-      <c r="Q31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>1,198</t>
+        </is>
+      </c>
       <c r="R31" t="inlineStr">
         <is>
           <t>Vivoactive HR 3.90.0.0</t>
@@ -4406,15 +4380,12 @@
         <v>5.183333333333334</v>
       </c>
       <c r="AF31" t="n">
-        <v>120</v>
+        <v>0.1414141414141414</v>
       </c>
       <c r="AG31" t="n">
-        <v>0.1414141414141414</v>
+        <v>0.8220988633359767</v>
       </c>
       <c r="AH31" t="n">
-        <v>0.8220988633359767</v>
-      </c>
-      <c r="AI31" t="n">
         <v>1.644197726671953</v>
       </c>
     </row>
@@ -4479,8 +4450,10 @@
           <t>00:43:58</t>
         </is>
       </c>
-      <c r="Q32" t="n">
-        <v>506</v>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>506</t>
+        </is>
       </c>
       <c r="R32" t="inlineStr">
         <is>
@@ -4533,15 +4506,12 @@
         <v>4.318181818181818</v>
       </c>
       <c r="AF32" t="n">
-        <v>44</v>
+        <v>0.1941747572815534</v>
       </c>
       <c r="AG32" t="n">
-        <v>0.1941747572815534</v>
+        <v>0.8050847457627118</v>
       </c>
       <c r="AH32" t="n">
-        <v>0.8050847457627118</v>
-      </c>
-      <c r="AI32" t="n">
         <v>0.5903954802259888</v>
       </c>
     </row>
@@ -4606,8 +4576,10 @@
           <t>01:17:20</t>
         </is>
       </c>
-      <c r="Q33" t="n">
-        <v>816</v>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>816</t>
+        </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
@@ -4660,15 +4632,12 @@
         <v>5.683544303797468</v>
       </c>
       <c r="AF33" t="n">
-        <v>79</v>
+        <v>0.2475247524752475</v>
       </c>
       <c r="AG33" t="n">
-        <v>0.2475247524752475</v>
+        <v>0.682370820668693</v>
       </c>
       <c r="AH33" t="n">
-        <v>0.682370820668693</v>
-      </c>
-      <c r="AI33" t="n">
         <v>0.8984549138804457</v>
       </c>
     </row>
@@ -4733,8 +4702,10 @@
           <t>00:54:04</t>
         </is>
       </c>
-      <c r="Q34" t="n">
-        <v>606</v>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>606</t>
+        </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
@@ -4787,15 +4758,12 @@
         <v>3.781818181818182</v>
       </c>
       <c r="AF34" t="n">
-        <v>55</v>
+        <v>0.11</v>
       </c>
       <c r="AG34" t="n">
-        <v>0.11</v>
+        <v>0.3753157704799711</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.3753157704799711</v>
-      </c>
-      <c r="AI34" t="n">
         <v>0.3440394562733068</v>
       </c>
     </row>
@@ -4860,8 +4828,10 @@
           <t>01:01:08</t>
         </is>
       </c>
-      <c r="Q35" t="n">
-        <v>729</v>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
@@ -4914,15 +4884,12 @@
         <v>4.065573770491803</v>
       </c>
       <c r="AF35" t="n">
-        <v>61</v>
+        <v>0.2685185185185185</v>
       </c>
       <c r="AG35" t="n">
-        <v>0.2685185185185185</v>
+        <v>0.5278842060451255</v>
       </c>
       <c r="AH35" t="n">
-        <v>0.5278842060451255</v>
-      </c>
-      <c r="AI35" t="n">
         <v>0.5366822761458776</v>
       </c>
     </row>
@@ -4987,8 +4954,10 @@
           <t>00:38:32</t>
         </is>
       </c>
-      <c r="Q36" t="n">
-        <v>470</v>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>470</t>
+        </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
@@ -5041,15 +5010,12 @@
         <v>5.282051282051282</v>
       </c>
       <c r="AF36" t="n">
-        <v>39</v>
+        <v>0.1296296296296296</v>
       </c>
       <c r="AG36" t="n">
-        <v>0.1296296296296296</v>
+        <v>0.5241730279898219</v>
       </c>
       <c r="AH36" t="n">
-        <v>0.5241730279898219</v>
-      </c>
-      <c r="AI36" t="n">
         <v>0.3407124681933842</v>
       </c>
     </row>
@@ -5114,8 +5080,10 @@
           <t>00:36:22</t>
         </is>
       </c>
-      <c r="Q37" t="n">
-        <v>411</v>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>411</t>
+        </is>
       </c>
       <c r="R37" t="inlineStr">
         <is>
@@ -5168,15 +5136,12 @@
         <v>6.25</v>
       </c>
       <c r="AF37" t="n">
-        <v>36</v>
+        <v>0.1414141414141414</v>
       </c>
       <c r="AG37" t="n">
-        <v>0.1414141414141414</v>
+        <v>0.4949406071271447</v>
       </c>
       <c r="AH37" t="n">
-        <v>0.4949406071271447</v>
-      </c>
-      <c r="AI37" t="n">
         <v>0.2969643642762868</v>
       </c>
     </row>
@@ -5241,8 +5206,10 @@
           <t>01:06:09</t>
         </is>
       </c>
-      <c r="Q38" t="n">
-        <v>806</v>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>806</t>
+        </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
@@ -5295,15 +5262,12 @@
         <v>4.878787878787879</v>
       </c>
       <c r="AF38" t="n">
-        <v>66</v>
+        <v>0.3518518518518519</v>
       </c>
       <c r="AG38" t="n">
-        <v>0.3518518518518519</v>
+        <v>0.6716729244889446</v>
       </c>
       <c r="AH38" t="n">
-        <v>0.6716729244889446</v>
-      </c>
-      <c r="AI38" t="n">
         <v>0.7388402169378391</v>
       </c>
     </row>
@@ -5368,8 +5332,10 @@
           <t>00:55:38</t>
         </is>
       </c>
-      <c r="Q39" t="n">
-        <v>737</v>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>737</t>
+        </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
@@ -5422,15 +5388,12 @@
         <v>4.545454545454546</v>
       </c>
       <c r="AF39" t="n">
-        <v>55</v>
+        <v>0.2612612612612613</v>
       </c>
       <c r="AG39" t="n">
-        <v>0.2612612612612613</v>
+        <v>0.5335040546308152</v>
       </c>
       <c r="AH39" t="n">
-        <v>0.5335040546308152</v>
-      </c>
-      <c r="AI39" t="n">
         <v>0.4890453834115805</v>
       </c>
     </row>
@@ -5495,8 +5458,10 @@
           <t>00:59:19</t>
         </is>
       </c>
-      <c r="Q40" t="n">
-        <v>698</v>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
@@ -5549,15 +5514,12 @@
         <v>4.338983050847458</v>
       </c>
       <c r="AF40" t="n">
-        <v>59</v>
+        <v>0.1855670103092784</v>
       </c>
       <c r="AG40" t="n">
-        <v>0.1855670103092784</v>
+        <v>1.002349256068912</v>
       </c>
       <c r="AH40" t="n">
-        <v>1.002349256068912</v>
-      </c>
-      <c r="AI40" t="n">
         <v>0.9856434351344295</v>
       </c>
     </row>
@@ -5622,8 +5584,10 @@
           <t>00:35:51</t>
         </is>
       </c>
-      <c r="Q41" t="n">
-        <v>477</v>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>477</t>
+        </is>
       </c>
       <c r="R41" t="inlineStr">
         <is>
@@ -5676,15 +5640,12 @@
         <v>5.837837837837838</v>
       </c>
       <c r="AF41" t="n">
-        <v>37</v>
+        <v>0.3716814159292036</v>
       </c>
       <c r="AG41" t="n">
-        <v>0.3716814159292036</v>
+        <v>0.4808548530721282</v>
       </c>
       <c r="AH41" t="n">
-        <v>0.4808548530721282</v>
-      </c>
-      <c r="AI41" t="n">
         <v>0.2965271593944791</v>
       </c>
     </row>
@@ -5749,8 +5710,10 @@
           <t>01:00:03</t>
         </is>
       </c>
-      <c r="Q42" t="n">
-        <v>761</v>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>761</t>
+        </is>
       </c>
       <c r="R42" t="inlineStr">
         <is>
@@ -5803,15 +5766,12 @@
         <v>4.233333333333333</v>
       </c>
       <c r="AF42" t="n">
-        <v>60</v>
+        <v>0.3490566037735849</v>
       </c>
       <c r="AG42" t="n">
-        <v>0.3490566037735849</v>
+        <v>0.5276277523888658</v>
       </c>
       <c r="AH42" t="n">
-        <v>0.5276277523888658</v>
-      </c>
-      <c r="AI42" t="n">
         <v>0.5276277523888658</v>
       </c>
     </row>
@@ -5876,8 +5836,10 @@
           <t>00:40:40</t>
         </is>
       </c>
-      <c r="Q43" t="n">
-        <v>508</v>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>508</t>
+        </is>
       </c>
       <c r="R43" t="inlineStr">
         <is>
@@ -5930,15 +5892,12 @@
         <v>4.926829268292683</v>
       </c>
       <c r="AF43" t="n">
-        <v>41</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="AG43" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.4580498866213152</v>
       </c>
       <c r="AH43" t="n">
-        <v>0.4580498866213152</v>
-      </c>
-      <c r="AI43" t="n">
         <v>0.3130007558578987</v>
       </c>
     </row>
@@ -6003,8 +5962,10 @@
           <t>00:34:53</t>
         </is>
       </c>
-      <c r="Q44" t="n">
-        <v>438</v>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>438</t>
+        </is>
       </c>
       <c r="R44" t="inlineStr">
         <is>
@@ -6057,15 +6018,12 @@
         <v>2.371428571428571</v>
       </c>
       <c r="AF44" t="n">
-        <v>35</v>
+        <v>0.3173076923076923</v>
       </c>
       <c r="AG44" t="n">
-        <v>0.3173076923076923</v>
+        <v>0.2862068965517242</v>
       </c>
       <c r="AH44" t="n">
-        <v>0.2862068965517242</v>
-      </c>
-      <c r="AI44" t="n">
         <v>0.1669540229885058</v>
       </c>
     </row>
@@ -6130,8 +6088,10 @@
           <t>00:47:07</t>
         </is>
       </c>
-      <c r="Q45" t="n">
-        <v>623</v>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>623</t>
+        </is>
       </c>
       <c r="R45" t="inlineStr">
         <is>
@@ -6184,15 +6144,12 @@
         <v>5.270833333333333</v>
       </c>
       <c r="AF45" t="n">
-        <v>48</v>
+        <v>0.1891891891891892</v>
       </c>
       <c r="AG45" t="n">
-        <v>0.1891891891891892</v>
+        <v>0.5212196126905645</v>
       </c>
       <c r="AH45" t="n">
-        <v>0.5212196126905645</v>
-      </c>
-      <c r="AI45" t="n">
         <v>0.4169756901524517</v>
       </c>
     </row>
@@ -6257,8 +6214,10 @@
           <t>00:20:23</t>
         </is>
       </c>
-      <c r="Q46" t="n">
-        <v>256</v>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>256</t>
+        </is>
       </c>
       <c r="R46" t="inlineStr">
         <is>
@@ -6311,15 +6270,12 @@
         <v>2.857142857142857</v>
       </c>
       <c r="AF46" t="n">
-        <v>21</v>
+        <v>0.1089108910891089</v>
       </c>
       <c r="AG46" t="n">
-        <v>0.1089108910891089</v>
+        <v>0.1180637544273908</v>
       </c>
       <c r="AH46" t="n">
-        <v>0.1180637544273908</v>
-      </c>
-      <c r="AI46" t="n">
         <v>0.04132231404958678</v>
       </c>
     </row>
@@ -6384,8 +6340,10 @@
           <t>00:25:25</t>
         </is>
       </c>
-      <c r="Q47" t="n">
-        <v>339</v>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>339</t>
+        </is>
       </c>
       <c r="R47" t="inlineStr">
         <is>
@@ -6438,15 +6396,12 @@
         <v>0.44</v>
       </c>
       <c r="AF47" t="n">
-        <v>25</v>
+        <v>0.03669724770642202</v>
       </c>
       <c r="AG47" t="n">
-        <v>0.03669724770642202</v>
+        <v>0.04937163375224416</v>
       </c>
       <c r="AH47" t="n">
-        <v>0.04937163375224416</v>
-      </c>
-      <c r="AI47" t="n">
         <v>0.02057151406343507</v>
       </c>
     </row>
@@ -6511,8 +6466,10 @@
           <t>00:37:31</t>
         </is>
       </c>
-      <c r="Q48" t="n">
-        <v>441</v>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>441</t>
+        </is>
       </c>
       <c r="R48" t="inlineStr">
         <is>
@@ -6565,15 +6522,12 @@
         <v>0.525</v>
       </c>
       <c r="AF48" t="n">
-        <v>40</v>
+        <v>0.18</v>
       </c>
       <c r="AG48" t="n">
-        <v>0.18</v>
+        <v>0.1314142678347935</v>
       </c>
       <c r="AH48" t="n">
-        <v>0.1314142678347935</v>
-      </c>
-      <c r="AI48" t="n">
         <v>0.08760951188986232</v>
       </c>
     </row>
@@ -6638,8 +6592,10 @@
           <t>00:53:49</t>
         </is>
       </c>
-      <c r="Q49" t="n">
-        <v>638</v>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>638</t>
+        </is>
       </c>
       <c r="R49" t="inlineStr">
         <is>
@@ -6692,15 +6648,12 @@
         <v>0.4035087719298245</v>
       </c>
       <c r="AF49" t="n">
-        <v>57</v>
+        <v>0.2574257425742574</v>
       </c>
       <c r="AG49" t="n">
-        <v>0.2574257425742574</v>
+        <v>0.08942457231726283</v>
       </c>
       <c r="AH49" t="n">
-        <v>0.08942457231726283</v>
-      </c>
-      <c r="AI49" t="n">
         <v>0.08495334370139969</v>
       </c>
     </row>
@@ -6765,8 +6718,10 @@
           <t>00:59:22</t>
         </is>
       </c>
-      <c r="Q50" t="n">
-        <v>756</v>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>756</t>
+        </is>
       </c>
       <c r="R50" t="inlineStr">
         <is>
@@ -6819,15 +6774,12 @@
         <v>4.483333333333333</v>
       </c>
       <c r="AF50" t="n">
-        <v>60</v>
+        <v>0.1296296296296296</v>
       </c>
       <c r="AG50" t="n">
-        <v>0.1296296296296296</v>
+        <v>0.5390781563126252</v>
       </c>
       <c r="AH50" t="n">
-        <v>0.5390781563126252</v>
-      </c>
-      <c r="AI50" t="n">
         <v>0.5390781563126252</v>
       </c>
     </row>
@@ -6892,8 +6844,10 @@
           <t>01:02:56</t>
         </is>
       </c>
-      <c r="Q51" t="n">
-        <v>749</v>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>749</t>
+        </is>
       </c>
       <c r="R51" t="inlineStr">
         <is>
@@ -6946,15 +6900,12 @@
         <v>4.11421875</v>
       </c>
       <c r="AF51" t="n">
-        <v>64</v>
+        <v>0.3009708737864077</v>
       </c>
       <c r="AG51" t="n">
-        <v>0.3009708737864077</v>
+        <v>0.5590920672668592</v>
       </c>
       <c r="AH51" t="n">
-        <v>0.5590920672668592</v>
-      </c>
-      <c r="AI51" t="n">
         <v>0.5963648717513165</v>
       </c>
     </row>
@@ -7019,8 +6970,10 @@
           <t>01:03:47</t>
         </is>
       </c>
-      <c r="Q52" t="n">
-        <v>771</v>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>771</t>
+        </is>
       </c>
       <c r="R52" t="inlineStr">
         <is>
@@ -7073,15 +7026,12 @@
         <v>4.1875</v>
       </c>
       <c r="AF52" t="n">
-        <v>64</v>
+        <v>0.219047619047619</v>
       </c>
       <c r="AG52" t="n">
-        <v>0.219047619047619</v>
+        <v>0.5861767279090114</v>
       </c>
       <c r="AH52" t="n">
-        <v>0.5861767279090114</v>
-      </c>
-      <c r="AI52" t="n">
         <v>0.6252551764362788</v>
       </c>
     </row>
@@ -7146,8 +7096,10 @@
           <t>00:54:34</t>
         </is>
       </c>
-      <c r="Q53" t="n">
-        <v>679</v>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>679</t>
+        </is>
       </c>
       <c r="R53" t="inlineStr">
         <is>
@@ -7200,15 +7152,12 @@
         <v>3.854545454545454</v>
       </c>
       <c r="AF53" t="n">
-        <v>55</v>
+        <v>0.3027522935779817</v>
       </c>
       <c r="AG53" t="n">
-        <v>0.3027522935779817</v>
+        <v>0.4789877993673746</v>
       </c>
       <c r="AH53" t="n">
-        <v>0.4789877993673746</v>
-      </c>
-      <c r="AI53" t="n">
         <v>0.4390721494200934</v>
       </c>
     </row>
@@ -7273,8 +7222,10 @@
           <t>00:41:05</t>
         </is>
       </c>
-      <c r="Q54" t="n">
-        <v>490</v>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>490</t>
+        </is>
       </c>
       <c r="R54" t="inlineStr">
         <is>
@@ -7327,15 +7278,12 @@
         <v>4.809523809523809</v>
       </c>
       <c r="AF54" t="n">
-        <v>42</v>
+        <v>0.330188679245283</v>
       </c>
       <c r="AG54" t="n">
-        <v>0.330188679245283</v>
+        <v>0.4584657285519745</v>
       </c>
       <c r="AH54" t="n">
-        <v>0.4584657285519745</v>
-      </c>
-      <c r="AI54" t="n">
         <v>0.3209260099863822</v>
       </c>
     </row>
@@ -7400,8 +7348,10 @@
           <t>00:48:33</t>
         </is>
       </c>
-      <c r="Q55" t="n">
-        <v>594</v>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>594</t>
+        </is>
       </c>
       <c r="R55" t="inlineStr">
         <is>
@@ -7454,15 +7404,12 @@
         <v>4.673469387755102</v>
       </c>
       <c r="AF55" t="n">
-        <v>49</v>
+        <v>0.2336448598130841</v>
       </c>
       <c r="AG55" t="n">
-        <v>0.2336448598130841</v>
+        <v>0.5088888888888888</v>
       </c>
       <c r="AH55" t="n">
-        <v>0.5088888888888888</v>
-      </c>
-      <c r="AI55" t="n">
         <v>0.4155925925925926</v>
       </c>
     </row>
@@ -7527,8 +7474,10 @@
           <t>00:42:19</t>
         </is>
       </c>
-      <c r="Q56" t="n">
-        <v>497</v>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>497</t>
+        </is>
       </c>
       <c r="R56" t="inlineStr">
         <is>
@@ -7581,15 +7530,12 @@
         <v>4.883720930232558</v>
       </c>
       <c r="AF56" t="n">
-        <v>43</v>
+        <v>0.23</v>
       </c>
       <c r="AG56" t="n">
-        <v>0.23</v>
+        <v>0.4672897196261682</v>
       </c>
       <c r="AH56" t="n">
-        <v>0.4672897196261682</v>
-      </c>
-      <c r="AI56" t="n">
         <v>0.3348909657320872</v>
       </c>
     </row>
@@ -7654,8 +7600,10 @@
           <t>00:42:25</t>
         </is>
       </c>
-      <c r="Q57" t="n">
-        <v>515</v>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>515</t>
+        </is>
       </c>
       <c r="R57" t="inlineStr">
         <is>
@@ -7708,15 +7656,12 @@
         <v>4.604651162790698</v>
       </c>
       <c r="AF57" t="n">
-        <v>43</v>
+        <v>0.2330097087378641</v>
       </c>
       <c r="AG57" t="n">
-        <v>0.2330097087378641</v>
+        <v>0.4441453566621804</v>
       </c>
       <c r="AH57" t="n">
-        <v>0.4441453566621804</v>
-      </c>
-      <c r="AI57" t="n">
         <v>0.3183041722745626</v>
       </c>
     </row>
@@ -7781,8 +7726,10 @@
           <t>00:25:57</t>
         </is>
       </c>
-      <c r="Q58" t="n">
-        <v>319</v>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>319</t>
+        </is>
       </c>
       <c r="R58" t="inlineStr">
         <is>
@@ -7835,15 +7782,12 @@
         <v>2.592592592592593</v>
       </c>
       <c r="AF58" t="n">
-        <v>27</v>
+        <v>0.2912621359223301</v>
       </c>
       <c r="AG58" t="n">
-        <v>0.2912621359223301</v>
+        <v>0.2353732347007398</v>
       </c>
       <c r="AH58" t="n">
-        <v>0.2353732347007398</v>
-      </c>
-      <c r="AI58" t="n">
         <v>0.1059179556153329</v>
       </c>
     </row>
@@ -7908,8 +7852,10 @@
           <t>00:57:51</t>
         </is>
       </c>
-      <c r="Q59" t="n">
-        <v>734</v>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>734</t>
+        </is>
       </c>
       <c r="R59" t="inlineStr">
         <is>
@@ -7962,15 +7908,12 @@
         <v>3.672413793103448</v>
       </c>
       <c r="AF59" t="n">
-        <v>58</v>
+        <v>0.2830188679245283</v>
       </c>
       <c r="AG59" t="n">
-        <v>0.2830188679245283</v>
+        <v>0.4901058444546709</v>
       </c>
       <c r="AH59" t="n">
-        <v>0.4901058444546709</v>
-      </c>
-      <c r="AI59" t="n">
         <v>0.4737689829728486</v>
       </c>
     </row>
@@ -8035,8 +7978,10 @@
           <t>00:56:26</t>
         </is>
       </c>
-      <c r="Q60" t="n">
-        <v>767</v>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>767</t>
+        </is>
       </c>
       <c r="R60" t="inlineStr">
         <is>
@@ -8089,15 +8034,12 @@
         <v>3.771929824561404</v>
       </c>
       <c r="AF60" t="n">
-        <v>57</v>
+        <v>0.1495327102803738</v>
       </c>
       <c r="AG60" t="n">
-        <v>0.1495327102803738</v>
+        <v>0.4862053369516056</v>
       </c>
       <c r="AH60" t="n">
-        <v>0.4862053369516056</v>
-      </c>
-      <c r="AI60" t="n">
         <v>0.4618950701040254</v>
       </c>
     </row>
@@ -8162,8 +8104,10 @@
           <t>00:55:04</t>
         </is>
       </c>
-      <c r="Q61" t="n">
-        <v>834</v>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>834</t>
+        </is>
       </c>
       <c r="R61" t="inlineStr">
         <is>
@@ -8216,15 +8160,12 @@
         <v>3.927272727272727</v>
       </c>
       <c r="AF61" t="n">
-        <v>55</v>
+        <v>0.25</v>
       </c>
       <c r="AG61" t="n">
-        <v>0.25</v>
+        <v>0.4871447902571042</v>
       </c>
       <c r="AH61" t="n">
-        <v>0.4871447902571042</v>
-      </c>
-      <c r="AI61" t="n">
         <v>0.4465493910690122</v>
       </c>
     </row>
@@ -8289,8 +8230,10 @@
           <t>00:26:55</t>
         </is>
       </c>
-      <c r="Q62" t="n">
-        <v>381</v>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>381</t>
+        </is>
       </c>
       <c r="R62" t="inlineStr">
         <is>
@@ -8343,15 +8286,12 @@
         <v>2.740740740740741</v>
       </c>
       <c r="AF62" t="n">
-        <v>27</v>
+        <v>0.2323232323232323</v>
       </c>
       <c r="AG62" t="n">
-        <v>0.2323232323232323</v>
+        <v>0.2429415627051871</v>
       </c>
       <c r="AH62" t="n">
-        <v>0.2429415627051871</v>
-      </c>
-      <c r="AI62" t="n">
         <v>0.1093237032173342</v>
       </c>
     </row>
@@ -8416,8 +8356,10 @@
           <t>00:27:32</t>
         </is>
       </c>
-      <c r="Q63" t="n">
-        <v>430</v>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>430</t>
+        </is>
       </c>
       <c r="R63" t="inlineStr">
         <is>
@@ -8470,15 +8412,12 @@
         <v>2.607142857142857</v>
       </c>
       <c r="AF63" t="n">
-        <v>28</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="AG63" t="n">
-        <v>0.462962962962963</v>
+        <v>0.2365521710952689</v>
       </c>
       <c r="AH63" t="n">
-        <v>0.2365521710952689</v>
-      </c>
-      <c r="AI63" t="n">
         <v>0.1103910131777922</v>
       </c>
     </row>
@@ -8543,8 +8482,10 @@
           <t>00:37:37</t>
         </is>
       </c>
-      <c r="Q64" t="n">
-        <v>626</v>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>626</t>
+        </is>
       </c>
       <c r="R64" t="inlineStr">
         <is>
@@ -8597,15 +8538,12 @@
         <v>2.5</v>
       </c>
       <c r="AF64" t="n">
-        <v>38</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AG64" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3112712975098296</v>
       </c>
       <c r="AH64" t="n">
-        <v>0.3112712975098296</v>
-      </c>
-      <c r="AI64" t="n">
         <v>0.1971384884228921</v>
       </c>
     </row>
@@ -8670,8 +8608,10 @@
           <t>00:26:56</t>
         </is>
       </c>
-      <c r="Q65" t="n">
-        <v>388</v>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>388</t>
+        </is>
       </c>
       <c r="R65" t="inlineStr">
         <is>
@@ -8724,15 +8664,12 @@
         <v>2.517241379310345</v>
       </c>
       <c r="AF65" t="n">
-        <v>29</v>
+        <v>0.05434782608695652</v>
       </c>
       <c r="AG65" t="n">
-        <v>0.05434782608695652</v>
+        <v>0.2428476380572189</v>
       </c>
       <c r="AH65" t="n">
-        <v>0.2428476380572189</v>
-      </c>
-      <c r="AI65" t="n">
         <v>0.1173763583943224</v>
       </c>
     </row>
@@ -8797,8 +8734,10 @@
           <t>00:26:48</t>
         </is>
       </c>
-      <c r="Q66" t="n">
-        <v>366</v>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>366</t>
+        </is>
       </c>
       <c r="R66" t="inlineStr">
         <is>
@@ -8851,15 +8790,12 @@
         <v>2.666666666666667</v>
       </c>
       <c r="AF66" t="n">
-        <v>27</v>
+        <v>0.2035398230088496</v>
       </c>
       <c r="AG66" t="n">
-        <v>0.2035398230088496</v>
+        <v>0.2445652173913044</v>
       </c>
       <c r="AH66" t="n">
-        <v>0.2445652173913044</v>
-      </c>
-      <c r="AI66" t="n">
         <v>0.110054347826087</v>
       </c>
     </row>
@@ -8924,8 +8860,10 @@
           <t>00:27:01</t>
         </is>
       </c>
-      <c r="Q67" t="n">
-        <v>387</v>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>387</t>
+        </is>
       </c>
       <c r="R67" t="inlineStr">
         <is>
@@ -8978,15 +8916,12 @@
         <v>2.607142857142857</v>
       </c>
       <c r="AF67" t="n">
-        <v>28</v>
+        <v>0.2809917355371901</v>
       </c>
       <c r="AG67" t="n">
-        <v>0.2809917355371901</v>
+        <v>0.2590489709013485</v>
       </c>
       <c r="AH67" t="n">
-        <v>0.2590489709013485</v>
-      </c>
-      <c r="AI67" t="n">
         <v>0.1208895197539626</v>
       </c>
     </row>
@@ -9051,8 +8986,10 @@
           <t>00:26:32</t>
         </is>
       </c>
-      <c r="Q68" t="n">
-        <v>350</v>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
       </c>
       <c r="R68" t="inlineStr">
         <is>
@@ -9105,15 +9042,12 @@
         <v>2.814814814814815</v>
       </c>
       <c r="AF68" t="n">
-        <v>27</v>
+        <v>0.4018691588785047</v>
       </c>
       <c r="AG68" t="n">
-        <v>0.4018691588785047</v>
+        <v>0.2722063037249284</v>
       </c>
       <c r="AH68" t="n">
-        <v>0.2722063037249284</v>
-      </c>
-      <c r="AI68" t="n">
         <v>0.1224928366762178</v>
       </c>
     </row>
@@ -9178,8 +9112,10 @@
           <t>00:27:39</t>
         </is>
       </c>
-      <c r="Q69" t="n">
-        <v>409</v>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>409</t>
+        </is>
       </c>
       <c r="R69" t="inlineStr">
         <is>
@@ -9232,15 +9168,12 @@
         <v>2.642857142857143</v>
       </c>
       <c r="AF69" t="n">
-        <v>28</v>
+        <v>0.5081967213114754</v>
       </c>
       <c r="AG69" t="n">
-        <v>0.5081967213114754</v>
+        <v>0.2714600146735143</v>
       </c>
       <c r="AH69" t="n">
-        <v>0.2714600146735143</v>
-      </c>
-      <c r="AI69" t="n">
         <v>0.1266813401809733</v>
       </c>
     </row>
@@ -9305,8 +9238,10 @@
           <t>00:25:36</t>
         </is>
       </c>
-      <c r="Q70" t="n">
-        <v>349</v>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>349</t>
+        </is>
       </c>
       <c r="R70" t="inlineStr">
         <is>
@@ -9359,15 +9294,12 @@
         <v>3.230769230769231</v>
       </c>
       <c r="AF70" t="n">
-        <v>26</v>
+        <v>0.4245283018867925</v>
       </c>
       <c r="AG70" t="n">
-        <v>0.4245283018867925</v>
+        <v>0.1124197002141328</v>
       </c>
       <c r="AH70" t="n">
-        <v>0.1124197002141328</v>
-      </c>
-      <c r="AI70" t="n">
         <v>0.0487152034261242</v>
       </c>
     </row>
@@ -9432,8 +9364,10 @@
           <t>00:27:09</t>
         </is>
       </c>
-      <c r="Q71" t="n">
-        <v>371</v>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>371</t>
+        </is>
       </c>
       <c r="R71" t="inlineStr">
         <is>
@@ -9486,15 +9420,12 @@
         <v>2.678571428571428</v>
       </c>
       <c r="AF71" t="n">
-        <v>28</v>
+        <v>0.4272727272727272</v>
       </c>
       <c r="AG71" t="n">
-        <v>0.4272727272727272</v>
+        <v>0.248015873015873</v>
       </c>
       <c r="AH71" t="n">
-        <v>0.248015873015873</v>
-      </c>
-      <c r="AI71" t="n">
         <v>0.1157407407407408</v>
       </c>
     </row>
@@ -9559,8 +9490,10 @@
           <t>00:33:51</t>
         </is>
       </c>
-      <c r="Q72" t="n">
-        <v>457</v>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>457</t>
+        </is>
       </c>
       <c r="R72" t="inlineStr">
         <is>
@@ -9613,15 +9546,12 @@
         <v>6.457142857142857</v>
       </c>
       <c r="AF72" t="n">
-        <v>35</v>
+        <v>0.2589285714285715</v>
       </c>
       <c r="AG72" t="n">
-        <v>0.2589285714285715</v>
+        <v>0.5422264875239923</v>
       </c>
       <c r="AH72" t="n">
-        <v>0.5422264875239923</v>
-      </c>
-      <c r="AI72" t="n">
         <v>0.3162987843889955</v>
       </c>
     </row>
@@ -9686,8 +9616,10 @@
           <t>00:26:17</t>
         </is>
       </c>
-      <c r="Q73" t="n">
-        <v>370</v>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>370</t>
+        </is>
       </c>
       <c r="R73" t="inlineStr">
         <is>
@@ -9740,15 +9672,12 @@
         <v>2.925925925925926</v>
       </c>
       <c r="AF73" t="n">
-        <v>27</v>
+        <v>0.1769911504424779</v>
       </c>
       <c r="AG73" t="n">
-        <v>0.1769911504424779</v>
+        <v>0.2762237762237762</v>
       </c>
       <c r="AH73" t="n">
-        <v>0.2762237762237762</v>
-      </c>
-      <c r="AI73" t="n">
         <v>0.1243006993006993</v>
       </c>
     </row>
@@ -9813,8 +9742,10 @@
           <t>00:41:20</t>
         </is>
       </c>
-      <c r="Q74" t="n">
-        <v>557</v>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>557</t>
+        </is>
       </c>
       <c r="R74" t="inlineStr">
         <is>
@@ -9867,15 +9798,12 @@
         <v>5.238095238095238</v>
       </c>
       <c r="AF74" t="n">
-        <v>42</v>
+        <v>0.3457943925233645</v>
       </c>
       <c r="AG74" t="n">
-        <v>0.3457943925233645</v>
+        <v>0.4795117698343505</v>
       </c>
       <c r="AH74" t="n">
-        <v>0.4795117698343505</v>
-      </c>
-      <c r="AI74" t="n">
         <v>0.3356582388840453</v>
       </c>
     </row>
@@ -9940,8 +9868,10 @@
           <t>00:25:58</t>
         </is>
       </c>
-      <c r="Q75" t="n">
-        <v>351</v>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>351</t>
+        </is>
       </c>
       <c r="R75" t="inlineStr">
         <is>
@@ -9994,15 +9924,12 @@
         <v>2.888888888888889</v>
       </c>
       <c r="AF75" t="n">
-        <v>27</v>
+        <v>0.2788461538461539</v>
       </c>
       <c r="AG75" t="n">
-        <v>0.2788461538461539</v>
+        <v>0.2575957727873184</v>
       </c>
       <c r="AH75" t="n">
-        <v>0.2575957727873184</v>
-      </c>
-      <c r="AI75" t="n">
         <v>0.1159180977542933</v>
       </c>
     </row>
@@ -10067,8 +9994,10 @@
           <t>00:45:54</t>
         </is>
       </c>
-      <c r="Q76" t="n">
-        <v>653</v>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>653</t>
+        </is>
       </c>
       <c r="R76" t="inlineStr">
         <is>
@@ -10121,15 +10050,12 @@
         <v>5.326086956521739</v>
       </c>
       <c r="AF76" t="n">
-        <v>46</v>
+        <v>0.2</v>
       </c>
       <c r="AG76" t="n">
-        <v>0.2</v>
+        <v>0.8572428271518544</v>
       </c>
       <c r="AH76" t="n">
-        <v>0.8572428271518544</v>
-      </c>
-      <c r="AI76" t="n">
         <v>0.6572195008164217</v>
       </c>
     </row>
@@ -10194,8 +10120,10 @@
           <t>00:45:57</t>
         </is>
       </c>
-      <c r="Q77" t="n">
-        <v>553</v>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>553</t>
+        </is>
       </c>
       <c r="R77" t="inlineStr">
         <is>
@@ -10248,15 +10176,12 @@
         <v>5.063829787234043</v>
       </c>
       <c r="AF77" t="n">
-        <v>47</v>
+        <v>0.3402061855670103</v>
       </c>
       <c r="AG77" t="n">
-        <v>0.3402061855670103</v>
+        <v>0.5149286023366508</v>
       </c>
       <c r="AH77" t="n">
-        <v>0.5149286023366508</v>
-      </c>
-      <c r="AI77" t="n">
         <v>0.4033607384970431</v>
       </c>
     </row>
@@ -10321,8 +10246,10 @@
           <t>00:27:40</t>
         </is>
       </c>
-      <c r="Q78" t="n">
-        <v>356</v>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>356</t>
+        </is>
       </c>
       <c r="R78" t="inlineStr">
         <is>
@@ -10375,15 +10302,12 @@
         <v>2.857142857142857</v>
       </c>
       <c r="AF78" t="n">
-        <v>28</v>
+        <v>0.1122448979591837</v>
       </c>
       <c r="AG78" t="n">
-        <v>0.1122448979591837</v>
+        <v>0.2635046113306982</v>
       </c>
       <c r="AH78" t="n">
-        <v>0.2635046113306982</v>
-      </c>
-      <c r="AI78" t="n">
         <v>0.1229688186209925</v>
       </c>
     </row>
@@ -10448,8 +10372,10 @@
           <t>00:27:29</t>
         </is>
       </c>
-      <c r="Q79" t="n">
-        <v>393</v>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>393</t>
+        </is>
       </c>
       <c r="R79" t="inlineStr">
         <is>
@@ -10502,15 +10428,12 @@
         <v>2.607142857142857</v>
       </c>
       <c r="AF79" t="n">
-        <v>28</v>
+        <v>0.2752293577981652</v>
       </c>
       <c r="AG79" t="n">
-        <v>0.2752293577981652</v>
+        <v>0.2407651715039578</v>
       </c>
       <c r="AH79" t="n">
-        <v>0.2407651715039578</v>
-      </c>
-      <c r="AI79" t="n">
         <v>0.1123570800351803</v>
       </c>
     </row>
@@ -10575,8 +10498,10 @@
           <t>00:25:50</t>
         </is>
       </c>
-      <c r="Q80" t="n">
-        <v>345</v>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
       </c>
       <c r="R80" t="inlineStr">
         <is>
@@ -10629,15 +10554,12 @@
         <v>3</v>
       </c>
       <c r="AF80" t="n">
-        <v>26</v>
+        <v>0.1386138613861386</v>
       </c>
       <c r="AG80" t="n">
-        <v>0.1386138613861386</v>
+        <v>0.3935418768920283</v>
       </c>
       <c r="AH80" t="n">
-        <v>0.3935418768920283</v>
-      </c>
-      <c r="AI80" t="n">
         <v>0.1705348133198789</v>
       </c>
     </row>
@@ -10702,8 +10624,10 @@
           <t>00:25:58</t>
         </is>
       </c>
-      <c r="Q81" t="n">
-        <v>372</v>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>372</t>
+        </is>
       </c>
       <c r="R81" t="inlineStr">
         <is>
@@ -10756,15 +10680,12 @@
         <v>2.653846153846154</v>
       </c>
       <c r="AF81" t="n">
-        <v>26</v>
+        <v>0.2522522522522522</v>
       </c>
       <c r="AG81" t="n">
-        <v>0.2522522522522522</v>
+        <v>0.2316991269308261</v>
       </c>
       <c r="AH81" t="n">
-        <v>0.2316991269308261</v>
-      </c>
-      <c r="AI81" t="n">
         <v>0.100402955003358</v>
       </c>
     </row>
@@ -10829,8 +10750,10 @@
           <t>00:18:35</t>
         </is>
       </c>
-      <c r="Q82" t="n">
-        <v>253</v>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>253</t>
+        </is>
       </c>
       <c r="R82" t="inlineStr">
         <is>
@@ -10883,15 +10806,12 @@
         <v>3.3</v>
       </c>
       <c r="AF82" t="n">
-        <v>20</v>
+        <v>0.2524271844660194</v>
       </c>
       <c r="AG82" t="n">
-        <v>0.2524271844660194</v>
+        <v>0.2168199737187911</v>
       </c>
       <c r="AH82" t="n">
-        <v>0.2168199737187911</v>
-      </c>
-      <c r="AI82" t="n">
         <v>0.07227332457293036</v>
       </c>
     </row>
@@ -10956,8 +10876,10 @@
           <t>00:39:23</t>
         </is>
       </c>
-      <c r="Q83" t="n">
-        <v>527</v>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>527</t>
+        </is>
       </c>
       <c r="R83" t="inlineStr">
         <is>
@@ -11010,15 +10932,12 @@
         <v>5.375</v>
       </c>
       <c r="AF83" t="n">
-        <v>40</v>
+        <v>0.1881188118811881</v>
       </c>
       <c r="AG83" t="n">
-        <v>0.1881188118811881</v>
+        <v>0.475453339230429</v>
       </c>
       <c r="AH83" t="n">
-        <v>0.475453339230429</v>
-      </c>
-      <c r="AI83" t="n">
         <v>0.316968892820286</v>
       </c>
     </row>
@@ -11083,8 +11002,10 @@
           <t>00:26:45</t>
         </is>
       </c>
-      <c r="Q84" t="n">
-        <v>394</v>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>394</t>
+        </is>
       </c>
       <c r="R84" t="inlineStr">
         <is>
@@ -11137,15 +11058,12 @@
         <v>2.678571428571428</v>
       </c>
       <c r="AF84" t="n">
-        <v>28</v>
+        <v>0.1926605504587156</v>
       </c>
       <c r="AG84" t="n">
-        <v>0.1926605504587156</v>
+        <v>0.2471984179301253</v>
       </c>
       <c r="AH84" t="n">
-        <v>0.2471984179301253</v>
-      </c>
-      <c r="AI84" t="n">
         <v>0.1153592617007251</v>
       </c>
     </row>
@@ -11210,8 +11128,10 @@
           <t>00:26:26</t>
         </is>
       </c>
-      <c r="Q85" t="n">
-        <v>377</v>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>377</t>
+        </is>
       </c>
       <c r="R85" t="inlineStr">
         <is>
@@ -11264,15 +11184,12 @@
         <v>2.592592592592593</v>
       </c>
       <c r="AF85" t="n">
-        <v>27</v>
+        <v>0.2524271844660194</v>
       </c>
       <c r="AG85" t="n">
-        <v>0.2524271844660194</v>
+        <v>0.3578732106339468</v>
       </c>
       <c r="AH85" t="n">
-        <v>0.3578732106339468</v>
-      </c>
-      <c r="AI85" t="n">
         <v>0.1610429447852761</v>
       </c>
     </row>
@@ -11337,8 +11254,10 @@
           <t>00:33:37</t>
         </is>
       </c>
-      <c r="Q86" t="n">
-        <v>465</v>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>465</t>
+        </is>
       </c>
       <c r="R86" t="inlineStr">
         <is>
@@ -11391,15 +11310,12 @@
         <v>2.371428571428571</v>
       </c>
       <c r="AF86" t="n">
-        <v>35</v>
+        <v>0.2772277227722773</v>
       </c>
       <c r="AG86" t="n">
-        <v>0.2772277227722773</v>
+        <v>0.4234693877551021</v>
       </c>
       <c r="AH86" t="n">
-        <v>0.4234693877551021</v>
-      </c>
-      <c r="AI86" t="n">
         <v>0.2470238095238095</v>
       </c>
     </row>
@@ -11464,8 +11380,10 @@
           <t>00:23:42</t>
         </is>
       </c>
-      <c r="Q87" t="n">
-        <v>340</v>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>340</t>
+        </is>
       </c>
       <c r="R87" t="inlineStr">
         <is>
@@ -11518,15 +11436,12 @@
         <v>3.125</v>
       </c>
       <c r="AF87" t="n">
-        <v>24</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG87" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2465483234714004</v>
       </c>
       <c r="AH87" t="n">
-        <v>0.2465483234714004</v>
-      </c>
-      <c r="AI87" t="n">
         <v>0.09861932938856018</v>
       </c>
     </row>
@@ -11591,8 +11506,10 @@
           <t>00:52:19</t>
         </is>
       </c>
-      <c r="Q88" t="n">
-        <v>710</v>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>710</t>
+        </is>
       </c>
       <c r="R88" t="inlineStr">
         <is>
@@ -11645,15 +11562,12 @@
         <v>4.075471698113208</v>
       </c>
       <c r="AF88" t="n">
-        <v>53</v>
+        <v>0.1326530612244898</v>
       </c>
       <c r="AG88" t="n">
-        <v>0.1326530612244898</v>
+        <v>0.4871447902571042</v>
       </c>
       <c r="AH88" t="n">
-        <v>0.4871447902571042</v>
-      </c>
-      <c r="AI88" t="n">
         <v>0.4303112313937754</v>
       </c>
     </row>
@@ -11718,7 +11632,11 @@
           <t>01:20:52</t>
         </is>
       </c>
-      <c r="Q89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>1,199</t>
+        </is>
+      </c>
       <c r="R89" t="inlineStr">
         <is>
           <t>Vivoactive HR 2.90.0.0</t>
@@ -11770,15 +11688,12 @@
         <v>6.010722891566265</v>
       </c>
       <c r="AF89" t="n">
-        <v>83</v>
+        <v>0.1224489795918367</v>
       </c>
       <c r="AG89" t="n">
-        <v>0.1224489795918367</v>
+        <v>0.7765791849568818</v>
       </c>
       <c r="AH89" t="n">
-        <v>0.7765791849568818</v>
-      </c>
-      <c r="AI89" t="n">
         <v>1.074267872523686</v>
       </c>
     </row>
@@ -11843,8 +11758,10 @@
           <t>02:16:45</t>
         </is>
       </c>
-      <c r="Q90" t="n">
-        <v>386</v>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
       </c>
       <c r="R90" t="inlineStr">
         <is>
@@ -11897,15 +11814,12 @@
         <v>0.06321167883211679</v>
       </c>
       <c r="AF90" t="n">
-        <v>137</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG90" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.03097281831187411</v>
       </c>
       <c r="AH90" t="n">
-        <v>0.03097281831187411</v>
-      </c>
-      <c r="AI90" t="n">
         <v>0.0707212684787792</v>
       </c>
     </row>
@@ -11970,8 +11884,10 @@
           <t>00:38:11</t>
         </is>
       </c>
-      <c r="Q91" t="n">
-        <v>542</v>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>542</t>
+        </is>
       </c>
       <c r="R91" t="inlineStr">
         <is>
@@ -12024,15 +11940,12 @@
         <v>5.261282051282051</v>
       </c>
       <c r="AF91" t="n">
-        <v>39</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG91" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4597168078146704</v>
       </c>
       <c r="AH91" t="n">
-        <v>0.4597168078146704</v>
-      </c>
-      <c r="AI91" t="n">
         <v>0.2988159250795358</v>
       </c>
     </row>
@@ -12097,8 +12010,10 @@
           <t>00:24:54</t>
         </is>
       </c>
-      <c r="Q92" t="n">
-        <v>398</v>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>398</t>
+        </is>
       </c>
       <c r="R92" t="inlineStr">
         <is>
@@ -12151,15 +12066,12 @@
         <v>3.0532</v>
       </c>
       <c r="AF92" t="n">
-        <v>25</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG92" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2391515493310775</v>
       </c>
       <c r="AH92" t="n">
-        <v>0.2391515493310775</v>
-      </c>
-      <c r="AI92" t="n">
         <v>0.09964647888794895</v>
       </c>
     </row>
@@ -12224,8 +12136,10 @@
           <t>01:07:10</t>
         </is>
       </c>
-      <c r="Q93" t="n">
-        <v>865</v>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>865</t>
+        </is>
       </c>
       <c r="R93" t="inlineStr">
         <is>
@@ -12278,15 +12192,12 @@
         <v>2.461029411764706</v>
       </c>
       <c r="AF93" t="n">
-        <v>68</v>
+        <v>0.1958762886597938</v>
       </c>
       <c r="AG93" t="n">
-        <v>0.1958762886597938</v>
+        <v>0.5291699604743083</v>
       </c>
       <c r="AH93" t="n">
-        <v>0.5291699604743083</v>
-      </c>
-      <c r="AI93" t="n">
         <v>0.599725955204216</v>
       </c>
     </row>
@@ -12351,8 +12262,10 @@
           <t>00:25:04</t>
         </is>
       </c>
-      <c r="Q94" t="n">
-        <v>398</v>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>398</t>
+        </is>
       </c>
       <c r="R94" t="inlineStr">
         <is>
@@ -12405,15 +12318,12 @@
         <v>2.66</v>
       </c>
       <c r="AF94" t="n">
-        <v>26</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG94" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2248447608829936</v>
       </c>
       <c r="AH94" t="n">
-        <v>0.2248447608829936</v>
-      </c>
-      <c r="AI94" t="n">
         <v>0.09743272971596389</v>
       </c>
     </row>
@@ -12478,8 +12388,10 @@
           <t>01:15:23</t>
         </is>
       </c>
-      <c r="Q95" t="n">
-        <v>923</v>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>923</t>
+        </is>
       </c>
       <c r="R95" t="inlineStr">
         <is>
@@ -12532,15 +12444,12 @@
         <v>5.069350649350649</v>
       </c>
       <c r="AF95" t="n">
-        <v>77</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG95" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.8547716025051459</v>
       </c>
       <c r="AH95" t="n">
-        <v>0.8547716025051459</v>
-      </c>
-      <c r="AI95" t="n">
         <v>1.096956889881604</v>
       </c>
     </row>
@@ -12605,8 +12514,10 @@
           <t>00:54:51</t>
         </is>
       </c>
-      <c r="Q96" t="n">
-        <v>712</v>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>712</t>
+        </is>
       </c>
       <c r="R96" t="inlineStr">
         <is>
@@ -12659,15 +12570,12 @@
         <v>3.77375</v>
       </c>
       <c r="AF96" t="n">
-        <v>56</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG96" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4760971433720826</v>
       </c>
       <c r="AH96" t="n">
-        <v>0.4760971433720826</v>
-      </c>
-      <c r="AI96" t="n">
         <v>0.4443573338139437</v>
       </c>
     </row>
@@ -12732,8 +12640,10 @@
           <t>01:09:14</t>
         </is>
       </c>
-      <c r="Q97" t="n">
-        <v>892</v>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>892</t>
+        </is>
       </c>
       <c r="R97" t="inlineStr">
         <is>
@@ -12786,15 +12696,12 @@
         <v>2.568169014084507</v>
       </c>
       <c r="AF97" t="n">
-        <v>71</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG97" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.5741183879093199</v>
       </c>
       <c r="AH97" t="n">
-        <v>0.5741183879093199</v>
-      </c>
-      <c r="AI97" t="n">
         <v>0.6793734256926952</v>
       </c>
     </row>
@@ -12859,8 +12766,10 @@
           <t>00:25:19</t>
         </is>
       </c>
-      <c r="Q98" t="n">
-        <v>388</v>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>388</t>
+        </is>
       </c>
       <c r="R98" t="inlineStr">
         <is>
@@ -12913,15 +12822,12 @@
         <v>2.683076923076923</v>
       </c>
       <c r="AF98" t="n">
-        <v>26</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG98" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2260311700093964</v>
       </c>
       <c r="AH98" t="n">
-        <v>0.2260311700093964</v>
-      </c>
-      <c r="AI98" t="n">
         <v>0.09794684033740511</v>
       </c>
     </row>
@@ -12986,8 +12892,10 @@
           <t>00:38:26</t>
         </is>
       </c>
-      <c r="Q99" t="n">
-        <v>453</v>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>453</t>
+        </is>
       </c>
       <c r="R99" t="inlineStr">
         <is>
@@ -13040,15 +12948,12 @@
         <v>5.561794871794872</v>
       </c>
       <c r="AF99" t="n">
-        <v>39</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG99" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4749195367065881</v>
       </c>
       <c r="AH99" t="n">
-        <v>0.4749195367065881</v>
-      </c>
-      <c r="AI99" t="n">
         <v>0.3086976988592823</v>
       </c>
     </row>
@@ -13113,8 +13018,10 @@
           <t>00:40:47</t>
         </is>
       </c>
-      <c r="Q100" t="n">
-        <v>567</v>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>567</t>
+        </is>
       </c>
       <c r="R100" t="inlineStr">
         <is>
@@ -13167,15 +13074,12 @@
         <v>2.831219512195122</v>
       </c>
       <c r="AF100" t="n">
-        <v>41</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG100" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.3637389151756338</v>
       </c>
       <c r="AH100" t="n">
-        <v>0.3637389151756338</v>
-      </c>
-      <c r="AI100" t="n">
         <v>0.2485549253700164</v>
       </c>
     </row>
@@ -13240,8 +13144,10 @@
           <t>00:26:42</t>
         </is>
       </c>
-      <c r="Q101" t="n">
-        <v>396</v>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>396</t>
+        </is>
       </c>
       <c r="R101" t="inlineStr">
         <is>
@@ -13294,15 +13200,12 @@
         <v>2.572592592592593</v>
       </c>
       <c r="AF101" t="n">
-        <v>27</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG101" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2258200851783218</v>
       </c>
       <c r="AH101" t="n">
-        <v>0.2258200851783218</v>
-      </c>
-      <c r="AI101" t="n">
         <v>0.1016190383302448</v>
       </c>
     </row>
@@ -13367,8 +13270,10 @@
           <t>00:47:00</t>
         </is>
       </c>
-      <c r="Q102" t="n">
-        <v>562</v>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>562</t>
+        </is>
       </c>
       <c r="R102" t="inlineStr">
         <is>
@@ -13421,15 +13326,12 @@
         <v>4.466808510638298</v>
       </c>
       <c r="AF102" t="n">
-        <v>47</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG102" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4599307715900627</v>
       </c>
       <c r="AH102" t="n">
-        <v>0.4599307715900627</v>
-      </c>
-      <c r="AI102" t="n">
         <v>0.3602791044122157</v>
       </c>
     </row>
@@ -13494,8 +13396,10 @@
           <t>00:37:42</t>
         </is>
       </c>
-      <c r="Q103" t="n">
-        <v>441</v>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>441</t>
+        </is>
       </c>
       <c r="R103" t="inlineStr">
         <is>
@@ -13548,15 +13452,12 @@
         <v>5.604736842105263</v>
       </c>
       <c r="AF103" t="n">
-        <v>38</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG103" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4663965838169276</v>
       </c>
       <c r="AH103" t="n">
-        <v>0.4663965838169276</v>
-      </c>
-      <c r="AI103" t="n">
         <v>0.2953845030840542</v>
       </c>
     </row>
@@ -13621,8 +13522,10 @@
           <t>01:13:50</t>
         </is>
       </c>
-      <c r="Q104" t="n">
-        <v>956</v>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>956</t>
+        </is>
       </c>
       <c r="R104" t="inlineStr">
         <is>
@@ -13675,15 +13578,12 @@
         <v>6.800657894736842</v>
       </c>
       <c r="AF104" t="n">
-        <v>76</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG104" t="n">
-        <v>0.2596153846153846</v>
+        <v>1.045958635204598</v>
       </c>
       <c r="AH104" t="n">
-        <v>1.045958635204598</v>
-      </c>
-      <c r="AI104" t="n">
         <v>1.324880937925824</v>
       </c>
     </row>
@@ -13748,8 +13648,10 @@
           <t>00:25:53</t>
         </is>
       </c>
-      <c r="Q105" t="n">
-        <v>397</v>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>397</t>
+        </is>
       </c>
       <c r="R105" t="inlineStr">
         <is>
@@ -13802,15 +13704,12 @@
         <v>2.680384615384615</v>
       </c>
       <c r="AF105" t="n">
-        <v>26</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG105" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2247992000258056</v>
       </c>
       <c r="AH105" t="n">
-        <v>0.2247992000258056</v>
-      </c>
-      <c r="AI105" t="n">
         <v>0.0974129866778491</v>
       </c>
     </row>
@@ -13875,8 +13774,10 @@
           <t>00:28:05</t>
         </is>
       </c>
-      <c r="Q106" t="n">
-        <v>384</v>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>384</t>
+        </is>
       </c>
       <c r="R106" t="inlineStr">
         <is>
@@ -13929,15 +13830,12 @@
         <v>2.511379310344827</v>
       </c>
       <c r="AF106" t="n">
-        <v>29</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG106" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2358942799766794</v>
       </c>
       <c r="AH106" t="n">
-        <v>0.2358942799766794</v>
-      </c>
-      <c r="AI106" t="n">
         <v>0.114015568655395</v>
       </c>
     </row>
@@ -14002,8 +13900,10 @@
           <t>00:26:32</t>
         </is>
       </c>
-      <c r="Q107" t="n">
-        <v>394</v>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>394</t>
+        </is>
       </c>
       <c r="R107" t="inlineStr">
         <is>
@@ -14056,15 +13956,12 @@
         <v>2.341851851851852</v>
       </c>
       <c r="AF107" t="n">
-        <v>27</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG107" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2050525359968867</v>
       </c>
       <c r="AH107" t="n">
-        <v>0.2050525359968867</v>
-      </c>
-      <c r="AI107" t="n">
         <v>0.09227364119859904</v>
       </c>
     </row>
@@ -14129,8 +14026,10 @@
           <t>00:48:02</t>
         </is>
       </c>
-      <c r="Q108" t="n">
-        <v>577</v>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>577</t>
+        </is>
       </c>
       <c r="R108" t="inlineStr">
         <is>
@@ -14183,15 +14082,12 @@
         <v>4.481020408163265</v>
       </c>
       <c r="AF108" t="n">
-        <v>49</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG108" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.480659355092927</v>
       </c>
       <c r="AH108" t="n">
-        <v>0.480659355092927</v>
-      </c>
-      <c r="AI108" t="n">
         <v>0.3925384733258904</v>
       </c>
     </row>
@@ -14256,8 +14152,10 @@
           <t>00:17:02</t>
         </is>
       </c>
-      <c r="Q109" t="n">
-        <v>266</v>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>266</t>
+        </is>
       </c>
       <c r="R109" t="inlineStr">
         <is>
@@ -14310,15 +14208,12 @@
         <v>4.136470588235293</v>
       </c>
       <c r="AF109" t="n">
-        <v>17</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG109" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2287052395355644</v>
       </c>
       <c r="AH109" t="n">
-        <v>0.2287052395355644</v>
-      </c>
-      <c r="AI109" t="n">
         <v>0.06479981786840992</v>
       </c>
     </row>
@@ -14383,8 +14278,10 @@
           <t>00:27:39</t>
         </is>
       </c>
-      <c r="Q110" t="n">
-        <v>398</v>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>398</t>
+        </is>
       </c>
       <c r="R110" t="inlineStr">
         <is>
@@ -14437,15 +14334,12 @@
         <v>2.573928571428571</v>
       </c>
       <c r="AF110" t="n">
-        <v>28</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG110" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2320198313051317</v>
       </c>
       <c r="AH110" t="n">
-        <v>0.2320198313051317</v>
-      </c>
-      <c r="AI110" t="n">
         <v>0.1082759212757281</v>
       </c>
     </row>
@@ -14510,8 +14404,10 @@
           <t>00:25:24</t>
         </is>
       </c>
-      <c r="Q111" t="n">
-        <v>400</v>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
       </c>
       <c r="R111" t="inlineStr">
         <is>
@@ -14564,15 +14460,12 @@
         <v>2.473076923076923</v>
       </c>
       <c r="AF111" t="n">
-        <v>26</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG111" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2051887545074512</v>
       </c>
       <c r="AH111" t="n">
-        <v>0.2051887545074512</v>
-      </c>
-      <c r="AI111" t="n">
         <v>0.08891512695322887</v>
       </c>
     </row>
@@ -14637,8 +14530,10 @@
           <t>00:47:23</t>
         </is>
       </c>
-      <c r="Q112" t="n">
-        <v>581</v>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>581</t>
+        </is>
       </c>
       <c r="R112" t="inlineStr">
         <is>
@@ -14691,15 +14586,12 @@
         <v>5.019375</v>
       </c>
       <c r="AF112" t="n">
-        <v>48</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG112" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.5274530408511756</v>
       </c>
       <c r="AH112" t="n">
-        <v>0.5274530408511756</v>
-      </c>
-      <c r="AI112" t="n">
         <v>0.4219624326809406</v>
       </c>
     </row>
@@ -14764,8 +14656,10 @@
           <t>00:26:46</t>
         </is>
       </c>
-      <c r="Q113" t="n">
-        <v>384</v>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>384</t>
+        </is>
       </c>
       <c r="R113" t="inlineStr">
         <is>
@@ -14818,15 +14712,12 @@
         <v>2.339259259259259</v>
       </c>
       <c r="AF113" t="n">
-        <v>27</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG113" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2048122446332447</v>
       </c>
       <c r="AH113" t="n">
-        <v>0.2048122446332447</v>
-      </c>
-      <c r="AI113" t="n">
         <v>0.09216551008496011</v>
       </c>
     </row>
@@ -14891,8 +14782,10 @@
           <t>01:16:04</t>
         </is>
       </c>
-      <c r="Q114" t="n">
-        <v>891</v>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>891</t>
+        </is>
       </c>
       <c r="R114" t="inlineStr">
         <is>
@@ -14945,15 +14838,12 @@
         <v>4.687272727272727</v>
       </c>
       <c r="AF114" t="n">
-        <v>77</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG114" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.7903126916002453</v>
       </c>
       <c r="AH114" t="n">
-        <v>0.7903126916002453</v>
-      </c>
-      <c r="AI114" t="n">
         <v>1.014234620886981</v>
       </c>
     </row>
@@ -15018,8 +14908,10 @@
           <t>00:43:07</t>
         </is>
       </c>
-      <c r="Q115" t="n">
-        <v>545</v>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>545</t>
+        </is>
       </c>
       <c r="R115" t="inlineStr">
         <is>
@@ -15072,15 +14964,12 @@
         <v>4.529333333333333</v>
       </c>
       <c r="AF115" t="n">
-        <v>45</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG115" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4525913754052494</v>
       </c>
       <c r="AH115" t="n">
-        <v>0.4525913754052494</v>
-      </c>
-      <c r="AI115" t="n">
         <v>0.339443531553937</v>
       </c>
     </row>
@@ -15145,8 +15034,10 @@
           <t>00:27:52</t>
         </is>
       </c>
-      <c r="Q116" t="n">
-        <v>387</v>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>387</t>
+        </is>
       </c>
       <c r="R116" t="inlineStr">
         <is>
@@ -15199,15 +15090,12 @@
         <v>2.235357142857143</v>
       </c>
       <c r="AF116" t="n">
-        <v>28</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG116" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.203181301736731</v>
       </c>
       <c r="AH116" t="n">
-        <v>0.203181301736731</v>
-      </c>
-      <c r="AI116" t="n">
         <v>0.0948179408104745</v>
       </c>
     </row>
@@ -15272,8 +15160,10 @@
           <t>00:46:24</t>
         </is>
       </c>
-      <c r="Q117" t="n">
-        <v>576</v>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>576</t>
+        </is>
       </c>
       <c r="R117" t="inlineStr">
         <is>
@@ -15326,15 +15216,12 @@
         <v>4.643191489361702</v>
       </c>
       <c r="AF117" t="n">
-        <v>47</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG117" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4777468858775367</v>
       </c>
       <c r="AH117" t="n">
-        <v>0.4777468858775367</v>
-      </c>
-      <c r="AI117" t="n">
         <v>0.3742350606040704</v>
       </c>
     </row>
@@ -15399,8 +15286,10 @@
           <t>00:56:49</t>
         </is>
       </c>
-      <c r="Q118" t="n">
-        <v>804</v>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>804</t>
+        </is>
       </c>
       <c r="R118" t="inlineStr">
         <is>
@@ -15453,15 +15342,12 @@
         <v>2.318965517241379</v>
       </c>
       <c r="AF118" t="n">
-        <v>58</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG118" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4346982967583465</v>
       </c>
       <c r="AH118" t="n">
-        <v>0.4346982967583465</v>
-      </c>
-      <c r="AI118" t="n">
         <v>0.4202083535330683</v>
       </c>
     </row>
@@ -15526,8 +15412,10 @@
           <t>00:28:20</t>
         </is>
       </c>
-      <c r="Q119" t="n">
-        <v>415</v>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>415</t>
+        </is>
       </c>
       <c r="R119" t="inlineStr">
         <is>
@@ -15580,15 +15468,12 @@
         <v>0.1275</v>
       </c>
       <c r="AF119" t="n">
-        <v>28</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG119" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.007635220394807195</v>
       </c>
       <c r="AH119" t="n">
-        <v>0.007635220394807195</v>
-      </c>
-      <c r="AI119" t="n">
         <v>0.003563102850910024</v>
       </c>
     </row>
@@ -15653,8 +15538,10 @@
           <t>00:25:59</t>
         </is>
       </c>
-      <c r="Q120" t="n">
-        <v>417</v>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>417</t>
+        </is>
       </c>
       <c r="R120" t="inlineStr">
         <is>
@@ -15707,15 +15594,12 @@
         <v>0.1330769230769231</v>
       </c>
       <c r="AF120" t="n">
-        <v>26</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG120" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.007401227833750455</v>
       </c>
       <c r="AH120" t="n">
-        <v>0.007401227833750455</v>
-      </c>
-      <c r="AI120" t="n">
         <v>0.00320719872795853</v>
       </c>
     </row>
@@ -15780,8 +15664,10 @@
           <t>00:26:51</t>
         </is>
       </c>
-      <c r="Q121" t="n">
-        <v>395</v>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>395</t>
+        </is>
       </c>
       <c r="R121" t="inlineStr">
         <is>
@@ -15834,15 +15720,12 @@
         <v>2.519642857142857</v>
       </c>
       <c r="AF121" t="n">
-        <v>28</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG121" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2293339401228749</v>
       </c>
       <c r="AH121" t="n">
-        <v>0.2293339401228749</v>
-      </c>
-      <c r="AI121" t="n">
         <v>0.107022505390675</v>
       </c>
     </row>
@@ -15907,8 +15790,10 @@
           <t>00:46:50</t>
         </is>
       </c>
-      <c r="Q122" t="n">
-        <v>589</v>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>589</t>
+        </is>
       </c>
       <c r="R122" t="inlineStr">
         <is>
@@ -15961,15 +15846,12 @@
         <v>4.533958333333334</v>
       </c>
       <c r="AF122" t="n">
-        <v>48</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG122" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4763290945304121</v>
       </c>
       <c r="AH122" t="n">
-        <v>0.4763290945304121</v>
-      </c>
-      <c r="AI122" t="n">
         <v>0.3810632756243297</v>
       </c>
     </row>
@@ -16034,8 +15916,10 @@
           <t>00:58:40</t>
         </is>
       </c>
-      <c r="Q123" t="n">
-        <v>825</v>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>825</t>
+        </is>
       </c>
       <c r="R123" t="inlineStr">
         <is>
@@ -16088,15 +15972,12 @@
         <v>2.286440677966102</v>
       </c>
       <c r="AF123" t="n">
-        <v>59</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG123" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4310317282806659</v>
       </c>
       <c r="AH123" t="n">
-        <v>0.4310317282806659</v>
-      </c>
-      <c r="AI123" t="n">
         <v>0.4238478661426547</v>
       </c>
     </row>
@@ -16161,8 +16042,10 @@
           <t>00:49:06</t>
         </is>
       </c>
-      <c r="Q124" t="n">
-        <v>579</v>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>579</t>
+        </is>
       </c>
       <c r="R124" t="inlineStr">
         <is>
@@ -16215,15 +16098,12 @@
         <v>4.3112</v>
       </c>
       <c r="AF124" t="n">
-        <v>50</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG124" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4725949311584671</v>
       </c>
       <c r="AH124" t="n">
-        <v>0.4725949311584671</v>
-      </c>
-      <c r="AI124" t="n">
         <v>0.3938291092987226</v>
       </c>
     </row>
@@ -16288,8 +16168,10 @@
           <t>00:26:24</t>
         </is>
       </c>
-      <c r="Q125" t="n">
-        <v>392</v>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>392</t>
+        </is>
       </c>
       <c r="R125" t="inlineStr">
         <is>
@@ -16342,15 +16224,12 @@
         <v>2.335172413793103</v>
       </c>
       <c r="AF125" t="n">
-        <v>29</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG125" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2199272538321642</v>
       </c>
       <c r="AH125" t="n">
-        <v>0.2199272538321642</v>
-      </c>
-      <c r="AI125" t="n">
         <v>0.106298172685546</v>
       </c>
     </row>
@@ -16415,8 +16294,10 @@
           <t>00:17:23</t>
         </is>
       </c>
-      <c r="Q126" t="n">
-        <v>273</v>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>273</t>
+        </is>
       </c>
       <c r="R126" t="inlineStr">
         <is>
@@ -16469,15 +16350,12 @@
         <v>3.487777777777778</v>
       </c>
       <c r="AF126" t="n">
-        <v>18</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG126" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2035535957460606</v>
       </c>
       <c r="AH126" t="n">
-        <v>0.2035535957460606</v>
-      </c>
-      <c r="AI126" t="n">
         <v>0.06106607872381816</v>
       </c>
     </row>
@@ -16542,8 +16420,10 @@
           <t>00:40:47</t>
         </is>
       </c>
-      <c r="Q127" t="n">
-        <v>435</v>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>435</t>
+        </is>
       </c>
       <c r="R127" t="inlineStr">
         <is>
@@ -16596,15 +16476,12 @@
         <v>4.928095238095238</v>
       </c>
       <c r="AF127" t="n">
-        <v>42</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG127" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4532574181539472</v>
       </c>
       <c r="AH127" t="n">
-        <v>0.4532574181539472</v>
-      </c>
-      <c r="AI127" t="n">
         <v>0.317280192707763</v>
       </c>
     </row>
@@ -16669,8 +16546,10 @@
           <t>00:28:14</t>
         </is>
       </c>
-      <c r="Q128" t="n">
-        <v>396</v>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>396</t>
+        </is>
       </c>
       <c r="R128" t="inlineStr">
         <is>
@@ -16723,15 +16602,12 @@
         <v>2.274482758620689</v>
       </c>
       <c r="AF128" t="n">
-        <v>29</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG128" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2139058243611363</v>
       </c>
       <c r="AH128" t="n">
-        <v>0.2139058243611363</v>
-      </c>
-      <c r="AI128" t="n">
         <v>0.1033878151078826</v>
       </c>
     </row>
@@ -16796,8 +16672,10 @@
           <t>00:26:51</t>
         </is>
       </c>
-      <c r="Q129" t="n">
-        <v>413</v>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>413</t>
+        </is>
       </c>
       <c r="R129" t="inlineStr">
         <is>
@@ -16850,15 +16728,12 @@
         <v>2.453793103448276</v>
       </c>
       <c r="AF129" t="n">
-        <v>29</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG129" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2276464378259062</v>
       </c>
       <c r="AH129" t="n">
-        <v>0.2276464378259062</v>
-      </c>
-      <c r="AI129" t="n">
         <v>0.1100291116158546</v>
       </c>
     </row>
@@ -16923,8 +16798,10 @@
           <t>00:46:39</t>
         </is>
       </c>
-      <c r="Q130" t="n">
-        <v>564</v>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>564</t>
+        </is>
       </c>
       <c r="R130" t="inlineStr">
         <is>
@@ -16977,15 +16854,12 @@
         <v>4.43468085106383</v>
       </c>
       <c r="AF130" t="n">
-        <v>47</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG130" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.4565726928216249</v>
       </c>
       <c r="AH130" t="n">
-        <v>0.4565726928216249</v>
-      </c>
-      <c r="AI130" t="n">
         <v>0.3576486093769395</v>
       </c>
     </row>
@@ -17050,8 +16924,10 @@
           <t>00:37:57</t>
         </is>
       </c>
-      <c r="Q131" t="n">
-        <v>516</v>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>516</t>
+        </is>
       </c>
       <c r="R131" t="inlineStr">
         <is>
@@ -17104,15 +16980,12 @@
         <v>4.147894736842106</v>
       </c>
       <c r="AF131" t="n">
-        <v>38</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG131" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.3974481819557215</v>
       </c>
       <c r="AH131" t="n">
-        <v>0.3974481819557215</v>
-      </c>
-      <c r="AI131" t="n">
         <v>0.2517171819052902</v>
       </c>
     </row>
@@ -17177,8 +17050,10 @@
           <t>00:26:48</t>
         </is>
       </c>
-      <c r="Q132" t="n">
-        <v>406</v>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>406</t>
+        </is>
       </c>
       <c r="R132" t="inlineStr">
         <is>
@@ -17231,15 +17106,12 @@
         <v>2.518888888888889</v>
       </c>
       <c r="AF132" t="n">
-        <v>27</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG132" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2213434876000781</v>
       </c>
       <c r="AH132" t="n">
-        <v>0.2213434876000781</v>
-      </c>
-      <c r="AI132" t="n">
         <v>0.09960456942003516</v>
       </c>
     </row>
@@ -17304,8 +17176,10 @@
           <t>00:18:47</t>
         </is>
       </c>
-      <c r="Q133" t="n">
-        <v>281</v>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>281</t>
+        </is>
       </c>
       <c r="R133" t="inlineStr">
         <is>
@@ -17358,15 +17232,12 @@
         <v>3.707368421052632</v>
       </c>
       <c r="AF133" t="n">
-        <v>19</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG133" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2282862328234379</v>
       </c>
       <c r="AH133" t="n">
-        <v>0.2282862328234379</v>
-      </c>
-      <c r="AI133" t="n">
         <v>0.07229064039408867</v>
       </c>
     </row>
@@ -17431,8 +17302,10 @@
           <t>00:26:49</t>
         </is>
       </c>
-      <c r="Q134" t="n">
-        <v>408</v>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>408</t>
+        </is>
       </c>
       <c r="R134" t="inlineStr">
         <is>
@@ -17485,15 +17358,12 @@
         <v>2.544444444444445</v>
       </c>
       <c r="AF134" t="n">
-        <v>27</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG134" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2227770931967054</v>
       </c>
       <c r="AH134" t="n">
-        <v>0.2227770931967054</v>
-      </c>
-      <c r="AI134" t="n">
         <v>0.1002496919385174</v>
       </c>
     </row>
@@ -17558,8 +17428,10 @@
           <t>00:28:32</t>
         </is>
       </c>
-      <c r="Q135" t="n">
-        <v>421</v>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>421</t>
+        </is>
       </c>
       <c r="R135" t="inlineStr">
         <is>
@@ -17612,15 +17484,12 @@
         <v>2.201724137931035</v>
       </c>
       <c r="AF135" t="n">
-        <v>29</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG135" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2074196796933372</v>
       </c>
       <c r="AH135" t="n">
-        <v>0.2074196796933372</v>
-      </c>
-      <c r="AI135" t="n">
         <v>0.100252845185113</v>
       </c>
     </row>
@@ -17685,8 +17554,10 @@
           <t>00:18:18</t>
         </is>
       </c>
-      <c r="Q136" t="n">
-        <v>285</v>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>285</t>
+        </is>
       </c>
       <c r="R136" t="inlineStr">
         <is>
@@ -17739,15 +17610,12 @@
         <v>3.57578947368421</v>
       </c>
       <c r="AF136" t="n">
-        <v>19</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG136" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2206775587098451</v>
       </c>
       <c r="AH136" t="n">
-        <v>0.2206775587098451</v>
-      </c>
-      <c r="AI136" t="n">
         <v>0.06988122692478427</v>
       </c>
     </row>
@@ -17812,8 +17680,10 @@
           <t>00:18:04</t>
         </is>
       </c>
-      <c r="Q137" t="n">
-        <v>281</v>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>281</t>
+        </is>
       </c>
       <c r="R137" t="inlineStr">
         <is>
@@ -17866,15 +17736,12 @@
         <v>4.2015</v>
       </c>
       <c r="AF137" t="n">
-        <v>20</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG137" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2577528296678016</v>
       </c>
       <c r="AH137" t="n">
-        <v>0.2577528296678016</v>
-      </c>
-      <c r="AI137" t="n">
         <v>0.08591760988926721</v>
       </c>
     </row>
@@ -17939,8 +17806,10 @@
           <t>00:19:14</t>
         </is>
       </c>
-      <c r="Q138" t="n">
-        <v>279</v>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>279</t>
+        </is>
       </c>
       <c r="R138" t="inlineStr">
         <is>
@@ -17993,15 +17862,12 @@
         <v>3.6225</v>
       </c>
       <c r="AF138" t="n">
-        <v>20</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG138" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2224507967699346</v>
       </c>
       <c r="AH138" t="n">
-        <v>0.2224507967699346</v>
-      </c>
-      <c r="AI138" t="n">
         <v>0.0741502655899782</v>
       </c>
     </row>
@@ -18066,8 +17932,10 @@
           <t>00:40:22</t>
         </is>
       </c>
-      <c r="Q139" t="n">
-        <v>573</v>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>573</t>
+        </is>
       </c>
       <c r="R139" t="inlineStr">
         <is>
@@ -18120,15 +17988,12 @@
         <v>4.130487804878048</v>
       </c>
       <c r="AF139" t="n">
-        <v>41</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG139" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.418065567295349</v>
       </c>
       <c r="AH139" t="n">
-        <v>0.418065567295349</v>
-      </c>
-      <c r="AI139" t="n">
         <v>0.2856781376518219</v>
       </c>
     </row>
@@ -18193,8 +18058,10 @@
           <t>00:35:33</t>
         </is>
       </c>
-      <c r="Q140" t="n">
-        <v>522</v>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>522</t>
+        </is>
       </c>
       <c r="R140" t="inlineStr">
         <is>
@@ -18247,15 +18114,12 @@
         <v>3.881388888888889</v>
       </c>
       <c r="AF140" t="n">
-        <v>36</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG140" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.3556918847367885</v>
       </c>
       <c r="AH140" t="n">
-        <v>0.3556918847367885</v>
-      </c>
-      <c r="AI140" t="n">
         <v>0.2134151308420731</v>
       </c>
     </row>
@@ -18320,8 +18184,10 @@
           <t>00:22:53</t>
         </is>
       </c>
-      <c r="Q141" t="n">
-        <v>343</v>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>343</t>
+        </is>
       </c>
       <c r="R141" t="inlineStr">
         <is>
@@ -18374,15 +18240,12 @@
         <v>3.185714285714286</v>
       </c>
       <c r="AF141" t="n">
-        <v>28</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG141" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2719512195121951</v>
       </c>
       <c r="AH141" t="n">
-        <v>0.2719512195121951</v>
-      </c>
-      <c r="AI141" t="n">
         <v>0.1269105691056911</v>
       </c>
     </row>
@@ -18447,8 +18310,10 @@
           <t>00:16:58</t>
         </is>
       </c>
-      <c r="Q142" t="n">
-        <v>267</v>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>267</t>
+        </is>
       </c>
       <c r="R142" t="inlineStr">
         <is>
@@ -18501,15 +18366,12 @@
         <v>4.168823529411765</v>
       </c>
       <c r="AF142" t="n">
-        <v>17</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG142" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2169401248928615</v>
       </c>
       <c r="AH142" t="n">
-        <v>0.2169401248928615</v>
-      </c>
-      <c r="AI142" t="n">
         <v>0.0614663687196441</v>
       </c>
     </row>
@@ -18574,8 +18436,10 @@
           <t>00:16:27</t>
         </is>
       </c>
-      <c r="Q143" t="n">
-        <v>267</v>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>267</t>
+        </is>
       </c>
       <c r="R143" t="inlineStr">
         <is>
@@ -18628,15 +18492,12 @@
         <v>4.266470588235294</v>
       </c>
       <c r="AF143" t="n">
-        <v>17</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG143" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2200345842308042</v>
       </c>
       <c r="AH143" t="n">
-        <v>0.2200345842308042</v>
-      </c>
-      <c r="AI143" t="n">
         <v>0.06234313219872786</v>
       </c>
     </row>
@@ -18701,8 +18562,10 @@
           <t>00:15:44</t>
         </is>
       </c>
-      <c r="Q144" t="n">
-        <v>224</v>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>224</t>
+        </is>
       </c>
       <c r="R144" t="inlineStr">
         <is>
@@ -18755,15 +18618,12 @@
         <v>3.904375</v>
       </c>
       <c r="AF144" t="n">
-        <v>16</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG144" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.1846695045524418</v>
       </c>
       <c r="AH144" t="n">
-        <v>0.1846695045524418</v>
-      </c>
-      <c r="AI144" t="n">
         <v>0.04924520121398447</v>
       </c>
     </row>
@@ -18828,8 +18688,10 @@
           <t>00:21:51</t>
         </is>
       </c>
-      <c r="Q145" t="n">
-        <v>343</v>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>343</t>
+        </is>
       </c>
       <c r="R145" t="inlineStr">
         <is>
@@ -18882,15 +18744,12 @@
         <v>3.029090909090909</v>
       </c>
       <c r="AF145" t="n">
-        <v>22</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG145" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2205235116979384</v>
       </c>
       <c r="AH145" t="n">
-        <v>0.2205235116979384</v>
-      </c>
-      <c r="AI145" t="n">
         <v>0.08085862095591073</v>
       </c>
     </row>
@@ -18955,8 +18814,10 @@
           <t>00:21:28</t>
         </is>
       </c>
-      <c r="Q146" t="n">
-        <v>341</v>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>341</t>
+        </is>
       </c>
       <c r="R146" t="inlineStr">
         <is>
@@ -19009,15 +18870,12 @@
         <v>4.049047619047619</v>
       </c>
       <c r="AF146" t="n">
-        <v>21</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG146" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2629820925988928</v>
       </c>
       <c r="AH146" t="n">
-        <v>0.2629820925988928</v>
-      </c>
-      <c r="AI146" t="n">
         <v>0.09204373240961246</v>
       </c>
     </row>
@@ -19082,8 +18940,10 @@
           <t>00:16:46</t>
         </is>
       </c>
-      <c r="Q147" t="n">
-        <v>258</v>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>258</t>
+        </is>
       </c>
       <c r="R147" t="inlineStr">
         <is>
@@ -19136,15 +18996,12 @@
         <v>4.165882352941176</v>
       </c>
       <c r="AF147" t="n">
-        <v>17</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG147" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.1270040529392776</v>
       </c>
       <c r="AH147" t="n">
-        <v>0.1270040529392776</v>
-      </c>
-      <c r="AI147" t="n">
         <v>0.03598448166612866</v>
       </c>
     </row>
@@ -19209,8 +19066,10 @@
           <t>00:29:56</t>
         </is>
       </c>
-      <c r="Q148" t="n">
-        <v>477</v>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>477</t>
+        </is>
       </c>
       <c r="R148" t="inlineStr">
         <is>
@@ -19263,15 +19122,12 @@
         <v>2.722</v>
       </c>
       <c r="AF148" t="n">
-        <v>30</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG148" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2623530167705455</v>
       </c>
       <c r="AH148" t="n">
-        <v>0.2623530167705455</v>
-      </c>
-      <c r="AI148" t="n">
         <v>0.1311765083852728</v>
       </c>
     </row>
@@ -19336,8 +19192,10 @@
           <t>00:27:20</t>
         </is>
       </c>
-      <c r="Q149" t="n">
-        <v>428</v>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>428</t>
+        </is>
       </c>
       <c r="R149" t="inlineStr">
         <is>
@@ -19390,15 +19248,12 @@
         <v>2.645</v>
       </c>
       <c r="AF149" t="n">
-        <v>28</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG149" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2391192044427224</v>
       </c>
       <c r="AH149" t="n">
-        <v>0.2391192044427224</v>
-      </c>
-      <c r="AI149" t="n">
         <v>0.1115889620732705</v>
       </c>
     </row>
@@ -19463,8 +19318,10 @@
           <t>00:29:04</t>
         </is>
       </c>
-      <c r="Q150" t="n">
-        <v>428</v>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>428</t>
+        </is>
       </c>
       <c r="R150" t="inlineStr">
         <is>
@@ -19517,15 +19374,12 @@
         <v>2.407586206896552</v>
       </c>
       <c r="AF150" t="n">
-        <v>29</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG150" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.226416318059474</v>
       </c>
       <c r="AH150" t="n">
-        <v>0.226416318059474</v>
-      </c>
-      <c r="AI150" t="n">
         <v>0.1094345537287458</v>
       </c>
     </row>
@@ -19590,8 +19444,10 @@
           <t>00:29:29</t>
         </is>
       </c>
-      <c r="Q151" t="n">
-        <v>420</v>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>420</t>
+        </is>
       </c>
       <c r="R151" t="inlineStr">
         <is>
@@ -19644,15 +19500,12 @@
         <v>1.718</v>
       </c>
       <c r="AF151" t="n">
-        <v>30</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG151" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.1674790407486839</v>
       </c>
       <c r="AH151" t="n">
-        <v>0.1674790407486839</v>
-      </c>
-      <c r="AI151" t="n">
         <v>0.08373952037434197</v>
       </c>
     </row>
@@ -19717,8 +19570,10 @@
           <t>00:21:00</t>
         </is>
       </c>
-      <c r="Q152" t="n">
-        <v>308</v>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>308</t>
+        </is>
       </c>
       <c r="R152" t="inlineStr">
         <is>
@@ -19771,15 +19626,12 @@
         <v>3.212857142857143</v>
       </c>
       <c r="AF152" t="n">
-        <v>21</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG152" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.2186396189118248</v>
       </c>
       <c r="AH152" t="n">
-        <v>0.2186396189118248</v>
-      </c>
-      <c r="AI152" t="n">
         <v>0.07652386661913865</v>
       </c>
     </row>
@@ -19844,8 +19696,10 @@
           <t>00:31:20</t>
         </is>
       </c>
-      <c r="Q153" t="n">
-        <v>386</v>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
       </c>
       <c r="R153" t="inlineStr">
         <is>
@@ -19898,15 +19752,12 @@
         <v>2.216875</v>
       </c>
       <c r="AF153" t="n">
-        <v>32</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG153" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.229230620092416</v>
       </c>
       <c r="AH153" t="n">
-        <v>0.229230620092416</v>
-      </c>
-      <c r="AI153" t="n">
         <v>0.1222563307159552</v>
       </c>
     </row>
@@ -19971,8 +19822,10 @@
           <t>00:20:27</t>
         </is>
       </c>
-      <c r="Q154" t="n">
-        <v>287</v>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>287</t>
+        </is>
       </c>
       <c r="R154" t="inlineStr">
         <is>
@@ -20025,15 +19878,12 @@
         <v>2.6145</v>
       </c>
       <c r="AF154" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AG154" t="n">
-        <v>0</v>
+        <v>0.1695690242241463</v>
       </c>
       <c r="AH154" t="n">
-        <v>0.1695690242241463</v>
-      </c>
-      <c r="AI154" t="n">
         <v>0.05652300807471543</v>
       </c>
     </row>
@@ -20098,8 +19948,10 @@
           <t>00:21:15</t>
         </is>
       </c>
-      <c r="Q155" t="n">
-        <v>351</v>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>351</t>
+        </is>
       </c>
       <c r="R155" t="inlineStr">
         <is>
@@ -20152,15 +20004,12 @@
         <v>2.974285714285714</v>
       </c>
       <c r="AF155" t="n">
-        <v>21</v>
+        <v>0.3879310344827586</v>
       </c>
       <c r="AG155" t="n">
-        <v>0.3879310344827586</v>
+        <v>0.2033004589395567</v>
       </c>
       <c r="AH155" t="n">
-        <v>0.2033004589395567</v>
-      </c>
-      <c r="AI155" t="n">
         <v>0.07115516062884483</v>
       </c>
     </row>
@@ -20225,8 +20074,10 @@
           <t>120:00:00</t>
         </is>
       </c>
-      <c r="Q156" t="n">
-        <v>401</v>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
       <c r="R156" t="inlineStr">
         <is>
@@ -20279,15 +20130,12 @@
         <v>7.831708830917668e-06</v>
       </c>
       <c r="AF156" t="n">
-        <v>750794</v>
+        <v>0.2596153846153846</v>
       </c>
       <c r="AG156" t="n">
-        <v>0.2596153846153846</v>
+        <v>0.02258411430327239</v>
       </c>
       <c r="AH156" t="n">
-        <v>0.02258411430327239</v>
-      </c>
-      <c r="AI156" t="n">
         <v>282.6002919035182</v>
       </c>
     </row>

</xml_diff>